<commit_message>
add labor adjustment to formatted table
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="basic" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,8 @@
     <externalReference r:id="rId22"/>
     <externalReference r:id="rId23"/>
     <externalReference r:id="rId24"/>
+    <externalReference r:id="rId25"/>
+    <externalReference r:id="rId26"/>
   </externalReferences>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="190">
   <si>
     <t xml:space="preserve">Note: the baseline model has Cobb-Douglas final good aggrgeator and balanced trade</t>
   </si>
@@ -317,6 +319,81 @@
   <si>
     <t xml:space="preserve">Volatility change due to specialization
 (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belgium and Luxembourg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colombia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portugal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States</t>
   </si>
   <si>
     <t xml:space="preserve">Note: Column (1) shows the percent change in average volatility as economies lowered their trading costs. Column (2) shows the contribution of diversification to the change in volatility in (1). Column (3) shows the contribution of specialization to the change in volatility in (1).</t>
@@ -2234,6 +2311,584 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="output_table"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="F2">
+            <v>1.53565969760448</v>
+          </cell>
+          <cell r="G2">
+            <v>-2.71755881791087</v>
+          </cell>
+          <cell r="H2">
+            <v>4.25321851551535</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="F3">
+            <v>-38.5279154522765</v>
+          </cell>
+          <cell r="G3">
+            <v>-63.1102312132425</v>
+          </cell>
+          <cell r="H3">
+            <v>24.5823157609659</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="F4">
+            <v>-50.4369578823248</v>
+          </cell>
+          <cell r="G4">
+            <v>-114.967667474995</v>
+          </cell>
+          <cell r="H4">
+            <v>64.5307095926705</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="F5">
+            <v>-60.3409836251069</v>
+          </cell>
+          <cell r="G5">
+            <v>-86.8373952493637</v>
+          </cell>
+          <cell r="H5">
+            <v>26.4964116242568</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="F6">
+            <v>1.4983505141899</v>
+          </cell>
+          <cell r="G6">
+            <v>0.404562364073804</v>
+          </cell>
+          <cell r="H6">
+            <v>1.09378815011609</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="F7">
+            <v>-21.2460741959909</v>
+          </cell>
+          <cell r="G7">
+            <v>-30.0166956657148</v>
+          </cell>
+          <cell r="H7">
+            <v>8.77062146972392</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="F8">
+            <v>-64.0181393545729</v>
+          </cell>
+          <cell r="G8">
+            <v>-47.7143781807209</v>
+          </cell>
+          <cell r="H8">
+            <v>-16.3037611738521</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="F9">
+            <v>-24.8789298589546</v>
+          </cell>
+          <cell r="G9">
+            <v>-60.6151655981537</v>
+          </cell>
+          <cell r="H9">
+            <v>35.7362357391991</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="F10">
+            <v>-15.7780180144079</v>
+          </cell>
+          <cell r="G10">
+            <v>6.41822020639214</v>
+          </cell>
+          <cell r="H10">
+            <v>-22.1962382208</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="F11">
+            <v>-27.7988506799051</v>
+          </cell>
+          <cell r="G11">
+            <v>-28.2268809748409</v>
+          </cell>
+          <cell r="H11">
+            <v>0.428030294935807</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="F12">
+            <v>-6.05592643701143</v>
+          </cell>
+          <cell r="G12">
+            <v>-9.83128374887882</v>
+          </cell>
+          <cell r="H12">
+            <v>3.77535731186739</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="F13">
+            <v>-11.2035330994139</v>
+          </cell>
+          <cell r="G13">
+            <v>-9.93230148713843</v>
+          </cell>
+          <cell r="H13">
+            <v>-1.27123161227549</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="F14">
+            <v>-60.1983780253013</v>
+          </cell>
+          <cell r="G14">
+            <v>-65.6128709674574</v>
+          </cell>
+          <cell r="H14">
+            <v>5.41449294215603</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="F15">
+            <v>-14.4078417117512</v>
+          </cell>
+          <cell r="G15">
+            <v>4.71884232358183</v>
+          </cell>
+          <cell r="H15">
+            <v>-19.126684035333</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="F16">
+            <v>-0.826092384415307</v>
+          </cell>
+          <cell r="G16">
+            <v>1.82713411767557</v>
+          </cell>
+          <cell r="H16">
+            <v>-2.65322650209088</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="F17">
+            <v>-52.0209504678687</v>
+          </cell>
+          <cell r="G17">
+            <v>-95.0974410260455</v>
+          </cell>
+          <cell r="H17">
+            <v>43.0764905581768</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="F18">
+            <v>-46.6285415670942</v>
+          </cell>
+          <cell r="G18">
+            <v>-139.472271334296</v>
+          </cell>
+          <cell r="H18">
+            <v>92.8437297672019</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="F19">
+            <v>-30.6682467622372</v>
+          </cell>
+          <cell r="G19">
+            <v>-77.2442100835886</v>
+          </cell>
+          <cell r="H19">
+            <v>46.5759633213514</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="F20">
+            <v>2.73429281907091</v>
+          </cell>
+          <cell r="G20">
+            <v>-35.3128491268408</v>
+          </cell>
+          <cell r="H20">
+            <v>38.0471419459117</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="F21">
+            <v>0.645602769649538</v>
+          </cell>
+          <cell r="G21">
+            <v>-2.53029015621022</v>
+          </cell>
+          <cell r="H21">
+            <v>3.17589292585977</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="F22">
+            <v>-8.52814823042821</v>
+          </cell>
+          <cell r="G22">
+            <v>-19.1323757812069</v>
+          </cell>
+          <cell r="H22">
+            <v>10.6042275507786</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="F23">
+            <v>-54.3889106351373</v>
+          </cell>
+          <cell r="G23">
+            <v>-26.2595934427098</v>
+          </cell>
+          <cell r="H23">
+            <v>-28.1293171924275</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="F24">
+            <v>-35.1188988311438</v>
+          </cell>
+          <cell r="G24">
+            <v>-37.9730664102412</v>
+          </cell>
+          <cell r="H24">
+            <v>2.85416757909741</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="F25">
+            <v>-43.8717707163064</v>
+          </cell>
+          <cell r="G25">
+            <v>-27.3801465095112</v>
+          </cell>
+          <cell r="H25">
+            <v>-16.4916242067951</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="F26">
+            <v>-0.433223766340495</v>
+          </cell>
+          <cell r="G26">
+            <v>2.53635681745116</v>
+          </cell>
+          <cell r="H26">
+            <v>-2.96958058379166</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="output_table"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="F2">
+            <v>1.24920886859601</v>
+          </cell>
+          <cell r="G2">
+            <v>-2.76100436543347</v>
+          </cell>
+          <cell r="H2">
+            <v>4.01021323402948</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="F3">
+            <v>-37.3535592295672</v>
+          </cell>
+          <cell r="G3">
+            <v>-63.6905108438777</v>
+          </cell>
+          <cell r="H3">
+            <v>26.3369516143105</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="F4">
+            <v>-50.5214820257963</v>
+          </cell>
+          <cell r="G4">
+            <v>-115.958047296187</v>
+          </cell>
+          <cell r="H4">
+            <v>65.4365652703909</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="F5">
+            <v>-60.8531517220489</v>
+          </cell>
+          <cell r="G5">
+            <v>-86.3291733470898</v>
+          </cell>
+          <cell r="H5">
+            <v>25.476021625041</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="F6">
+            <v>1.53195692063427</v>
+          </cell>
+          <cell r="G6">
+            <v>0.360723902908225</v>
+          </cell>
+          <cell r="H6">
+            <v>1.17123301772604</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="F7">
+            <v>-21.2743927968265</v>
+          </cell>
+          <cell r="G7">
+            <v>-29.5645696806361</v>
+          </cell>
+          <cell r="H7">
+            <v>8.29017688380957</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="F8">
+            <v>-64.1669041955435</v>
+          </cell>
+          <cell r="G8">
+            <v>-48.1580906373406</v>
+          </cell>
+          <cell r="H8">
+            <v>-16.0088135582029</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="F9">
+            <v>-24.8640073764381</v>
+          </cell>
+          <cell r="G9">
+            <v>-61.1969865804073</v>
+          </cell>
+          <cell r="H9">
+            <v>36.3329792039692</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="F10">
+            <v>-15.5584347216418</v>
+          </cell>
+          <cell r="G10">
+            <v>6.80416134993578</v>
+          </cell>
+          <cell r="H10">
+            <v>-22.3625960715776</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="F11">
+            <v>-27.9334177059314</v>
+          </cell>
+          <cell r="G11">
+            <v>-28.2076092078725</v>
+          </cell>
+          <cell r="H11">
+            <v>0.274191501941107</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="F12">
+            <v>-5.48861839313903</v>
+          </cell>
+          <cell r="G12">
+            <v>-10.7663957650113</v>
+          </cell>
+          <cell r="H12">
+            <v>5.27777737187224</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="F13">
+            <v>-11.2192688765699</v>
+          </cell>
+          <cell r="G13">
+            <v>-9.92610155153194</v>
+          </cell>
+          <cell r="H13">
+            <v>-1.29316732503796</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="F14">
+            <v>-59.8161223001668</v>
+          </cell>
+          <cell r="G14">
+            <v>-67.2050236265695</v>
+          </cell>
+          <cell r="H14">
+            <v>7.38890132640277</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="F15">
+            <v>-14.1849952522035</v>
+          </cell>
+          <cell r="G15">
+            <v>5.23557686980738</v>
+          </cell>
+          <cell r="H15">
+            <v>-19.4205721220108</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="F16">
+            <v>-0.940976731782397</v>
+          </cell>
+          <cell r="G16">
+            <v>1.9212893334437</v>
+          </cell>
+          <cell r="H16">
+            <v>-2.8622660652261</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="F17">
+            <v>-52.087796342518</v>
+          </cell>
+          <cell r="G17">
+            <v>-93.7942610951611</v>
+          </cell>
+          <cell r="H17">
+            <v>41.7064647526431</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="F18">
+            <v>-47.1785356250076</v>
+          </cell>
+          <cell r="G18">
+            <v>-141.762503623923</v>
+          </cell>
+          <cell r="H18">
+            <v>94.5839679989157</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="F19">
+            <v>-30.1867219949592</v>
+          </cell>
+          <cell r="G19">
+            <v>-77.2243565108896</v>
+          </cell>
+          <cell r="H19">
+            <v>47.0376345159305</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="F20">
+            <v>1.72108421710482</v>
+          </cell>
+          <cell r="G20">
+            <v>-35.5889673796901</v>
+          </cell>
+          <cell r="H20">
+            <v>37.3100515967949</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="F21">
+            <v>0.683610189736178</v>
+          </cell>
+          <cell r="G21">
+            <v>-2.5002919845191</v>
+          </cell>
+          <cell r="H21">
+            <v>3.18390217425528</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="F22">
+            <v>-8.86283645070318</v>
+          </cell>
+          <cell r="G22">
+            <v>-19.8806587417992</v>
+          </cell>
+          <cell r="H22">
+            <v>11.0178222910961</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="F23">
+            <v>-54.2789119406964</v>
+          </cell>
+          <cell r="G23">
+            <v>-26.4513289680599</v>
+          </cell>
+          <cell r="H23">
+            <v>-27.8275829726364</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="F24">
+            <v>-35.6306450415239</v>
+          </cell>
+          <cell r="G24">
+            <v>-38.2452330189464</v>
+          </cell>
+          <cell r="H24">
+            <v>2.61458797742249</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="F25">
+            <v>-44.1726536210684</v>
+          </cell>
+          <cell r="G25">
+            <v>-26.94770311953</v>
+          </cell>
+          <cell r="H25">
+            <v>-17.2249505015384</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="F26">
+            <v>-0.441011625162661</v>
+          </cell>
+          <cell r="G26">
+            <v>2.7479450706726</v>
+          </cell>
+          <cell r="H26">
+            <v>-3.18895669583526</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -32771,7 +33426,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32783,7 +33438,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32828,9 +33483,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A7" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="B7" s="17" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F2,1),"0.0"),"%")</f>
@@ -32858,9 +33512,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A8" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="B8" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F3,1),"0.0"),"%")</f>
@@ -32888,9 +33541,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A9" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="B9" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F4,1),"0.0"),"%")</f>
@@ -32918,9 +33570,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A10" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="B10" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F5,1),"0.0"),"%")</f>
@@ -32948,9 +33599,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A11" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="B11" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F6,1),"0.0"),"%")</f>
@@ -32978,9 +33628,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A12" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="B12" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F7,1),"0.0"),"%")</f>
@@ -33008,9 +33657,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A13" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="B13" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F8,1),"0.0"),"%")</f>
@@ -33038,9 +33686,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A14" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="B14" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F9,1),"0.0"),"%")</f>
@@ -33068,9 +33715,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A15" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="B15" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F10,1),"0.0"),"%")</f>
@@ -33098,9 +33744,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A16" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="B16" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F11,1),"0.0"),"%")</f>
@@ -33128,9 +33773,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A17" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="B17" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F12,1),"0.0"),"%")</f>
@@ -33158,9 +33802,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A18" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="B18" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F13,1),"0.0"),"%")</f>
@@ -33188,9 +33831,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A19" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="B19" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F14,1),"0.0"),"%")</f>
@@ -33218,9 +33860,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A20" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="B20" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F15,1),"0.0"),"%")</f>
@@ -33248,9 +33889,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A21" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B21" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F16,1),"0.0"),"%")</f>
@@ -33278,9 +33918,8 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A22" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="B22" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F17,1),"0.0"),"%")</f>
@@ -33308,9 +33947,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A23" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="B23" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F18,1),"0.0"),"%")</f>
@@ -33338,9 +33976,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A24" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="B24" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F19,1),"0.0"),"%")</f>
@@ -33368,9 +34005,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A25" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="B25" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F20,1),"0.0"),"%")</f>
@@ -33398,9 +34034,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A26" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="B26" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F21,1),"0.0"),"%")</f>
@@ -33428,9 +34063,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A27" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="B27" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F22,1),"0.0"),"%")</f>
@@ -33458,9 +34092,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A28" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="B28" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F23,1),"0.0"),"%")</f>
@@ -33488,9 +34121,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A29" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="B29" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F24,1),"0.0"),"%")</f>
@@ -33518,9 +34150,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A30" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="B30" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F25,1),"0.0"),"%")</f>
@@ -33548,9 +34179,8 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A31" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="B31" s="25" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([10]output_table!F26,1),"0.0"),"%")</f>
@@ -33579,7 +34209,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -33606,7 +34236,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33629,22 +34259,21 @@
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="13" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A6" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="B6" s="44" t="n">
         <f aca="false">ROUND([1]output_table!B2,6)</f>
@@ -33664,9 +34293,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A7" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="B7" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B3,6)</f>
@@ -33686,9 +34314,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A8" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="B8" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B4,6)</f>
@@ -33708,9 +34335,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A9" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="B9" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B5,6)</f>
@@ -33730,9 +34356,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A10" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="B10" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B6,6)</f>
@@ -33752,9 +34377,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A11" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="B11" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B7,6)</f>
@@ -33774,9 +34398,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A12" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="B12" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B8,6)</f>
@@ -33796,9 +34419,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A13" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="B13" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B9,6)</f>
@@ -33818,9 +34440,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A14" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="B14" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B10,6)</f>
@@ -33840,9 +34461,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A15" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="B15" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B11,6)</f>
@@ -33862,9 +34482,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A16" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="B16" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B12,6)</f>
@@ -33884,9 +34503,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A17" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="B17" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B13,6)</f>
@@ -33906,9 +34524,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A18" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="B18" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B14,6)</f>
@@ -33928,9 +34545,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A19" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="B19" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B15,6)</f>
@@ -33950,9 +34566,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A20" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B20" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B16,6)</f>
@@ -33972,9 +34587,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A21" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="B21" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B17,6)</f>
@@ -33994,9 +34608,8 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A22" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="B22" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B18,6)</f>
@@ -34016,9 +34629,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A23" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="B23" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B19,6)</f>
@@ -34038,9 +34650,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A24" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="B24" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B20,6)</f>
@@ -34060,9 +34671,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A25" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="B25" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B21,6)</f>
@@ -34082,9 +34692,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A26" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="B26" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B22,6)</f>
@@ -34104,9 +34713,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A27" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="B27" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B23,6)</f>
@@ -34126,9 +34734,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A28" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="B28" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B24,6)</f>
@@ -34148,9 +34755,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A29" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="B29" s="47" t="n">
         <f aca="false">ROUND([1]output_table!B25,6)</f>
@@ -34170,9 +34776,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A30" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="B30" s="51" t="n">
         <f aca="false">ROUND([1]output_table!B26,6)</f>
@@ -34193,7 +34798,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -34227,26 +34832,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K1" s="0" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.0451017</v>
@@ -34258,12 +34863,12 @@
         <v>0.53</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.0675627</v>
@@ -34275,12 +34880,12 @@
         <v>4.27</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.1177053</v>
@@ -34292,12 +34897,12 @@
         <v>4.61</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.0096435</v>
@@ -34311,19 +34916,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K7" s="0" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="54"/>
       <c r="K9" s="0" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="54"/>
       <c r="K10" s="0" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34332,422 +34937,422 @@
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="54"/>
       <c r="K12" s="0" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K13" s="0" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K14" s="0" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K15" s="0" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K17" s="0" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K19" s="0" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K20" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K22" s="0" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K23" s="0" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K24" s="0" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K25" s="0" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K27" s="0" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K28" s="0" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K30" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K31" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K32" s="0" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K33" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K34" s="0" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K35" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K37" s="0" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K39" s="0" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K40" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K42" s="0" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K43" s="0" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K44" s="0" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K45" s="0" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K47" s="0" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K48" s="0" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K50" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K51" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K52" s="0" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K53" s="0" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K54" s="0" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K55" s="0" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K56" s="0" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K57" s="0" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K58" s="0" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K59" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K60" s="0" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K62" s="0" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K63" s="0" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K64" s="0" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K65" s="0" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K67" s="0" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K69" s="0" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K70" s="0" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K72" s="0" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K73" s="0" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K74" s="0" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K75" s="0" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K77" s="0" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K78" s="0" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K80" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K81" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K82" s="0" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K83" s="0" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K84" s="0" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K85" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K87" s="0" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K89" s="0" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K90" s="0" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K92" s="0" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K93" s="0" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K94" s="0" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K95" s="0" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K97" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K98" s="0" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K100" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K101" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K102" s="0" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K103" s="0" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K104" s="0" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K105" s="0" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K106" s="0" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K107" s="0" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K108" s="0" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K109" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K110" s="0" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K112" s="0" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K113" s="0" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K114" s="0" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K115" s="0" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K116" s="0" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K117" s="0" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -34769,7 +35374,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -34821,7 +35426,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34855,9 +35460,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A6" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="B6" s="17" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F2,1),"0.0"),"%")</f>
@@ -34873,9 +35477,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A7" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="B7" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F3,1),"0.0"),"%")</f>
@@ -34891,9 +35494,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A8" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="B8" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F4,1),"0.0"),"%")</f>
@@ -34909,9 +35511,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A9" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="B9" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F5,1),"0.0"),"%")</f>
@@ -34927,9 +35528,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A10" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="B10" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F6,1),"0.0"),"%")</f>
@@ -34945,9 +35545,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A11" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="B11" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F7,1),"0.0"),"%")</f>
@@ -34967,9 +35566,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A12" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="B12" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F8,1),"0.0"),"%")</f>
@@ -34985,9 +35583,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A13" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="B13" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F9,1),"0.0"),"%")</f>
@@ -35003,9 +35600,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A14" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="B14" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F10,1),"0.0"),"%")</f>
@@ -35021,9 +35617,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A15" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="B15" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F11,1),"0.0"),"%")</f>
@@ -35039,9 +35634,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A16" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="B16" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F12,1),"0.0"),"%")</f>
@@ -35057,9 +35651,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A17" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="B17" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F13,1),"0.0"),"%")</f>
@@ -35075,9 +35668,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A18" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="B18" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F14,1),"0.0"),"%")</f>
@@ -35093,9 +35685,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A19" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="B19" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F15,1),"0.0"),"%")</f>
@@ -35111,9 +35702,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A20" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B20" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F16,1),"0.0"),"%")</f>
@@ -35129,9 +35719,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A21" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="B21" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F17,1),"0.0"),"%")</f>
@@ -35147,9 +35736,8 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A22" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="B22" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F18,1),"0.0"),"%")</f>
@@ -35165,9 +35753,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A23" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="B23" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F19,1),"0.0"),"%")</f>
@@ -35183,9 +35770,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A24" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="B24" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F20,1),"0.0"),"%")</f>
@@ -35201,9 +35787,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A25" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="B25" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F21,1),"0.0"),"%")</f>
@@ -35219,9 +35804,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A26" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="B26" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F22,1),"0.0"),"%")</f>
@@ -35237,9 +35821,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A27" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="B27" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F23,1),"0.0"),"%")</f>
@@ -35255,9 +35838,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A28" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="B28" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F24,1),"0.0"),"%")</f>
@@ -35273,9 +35855,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A29" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="B29" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F25,1),"0.0"),"%")</f>
@@ -35291,9 +35872,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A30" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="B30" s="25" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([1]output_table!F26,1),"0.0"),"%")</f>
@@ -35310,7 +35890,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -35333,7 +35913,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35367,9 +35947,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A6" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="B6" s="17" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F2,1),"0.0"),"%")</f>
@@ -35385,9 +35964,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A7" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="B7" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F3,1),"0.0"),"%")</f>
@@ -35403,9 +35981,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A8" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="B8" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F4,1),"0.0"),"%")</f>
@@ -35421,9 +35998,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A9" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="B9" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F5,1),"0.0"),"%")</f>
@@ -35439,9 +36015,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A10" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="B10" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F6,1),"0.0"),"%")</f>
@@ -35457,9 +36032,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A11" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="B11" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F7,1),"0.0"),"%")</f>
@@ -35475,9 +36049,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A12" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="B12" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F8,1),"0.0"),"%")</f>
@@ -35493,9 +36066,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A13" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="B13" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F9,1),"0.0"),"%")</f>
@@ -35511,9 +36083,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A14" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="B14" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F10,1),"0.0"),"%")</f>
@@ -35529,9 +36100,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A15" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="B15" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F11,1),"0.0"),"%")</f>
@@ -35547,9 +36117,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A16" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="B16" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F12,1),"0.0"),"%")</f>
@@ -35565,9 +36134,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A17" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="B17" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F13,1),"0.0"),"%")</f>
@@ -35583,9 +36151,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A18" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="B18" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F14,1),"0.0"),"%")</f>
@@ -35601,9 +36168,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A19" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="B19" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F15,1),"0.0"),"%")</f>
@@ -35619,9 +36185,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A20" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B20" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F16,1),"0.0"),"%")</f>
@@ -35637,9 +36202,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A21" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="B21" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F17,1),"0.0"),"%")</f>
@@ -35655,9 +36219,8 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A22" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="B22" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F18,1),"0.0"),"%")</f>
@@ -35673,9 +36236,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A23" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="B23" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F19,1),"0.0"),"%")</f>
@@ -35691,9 +36253,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A24" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="B24" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F20,1),"0.0"),"%")</f>
@@ -35709,9 +36270,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A25" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="B25" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F21,1),"0.0"),"%")</f>
@@ -35727,9 +36287,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A26" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="B26" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F22,1),"0.0"),"%")</f>
@@ -35745,9 +36304,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A27" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="B27" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F23,1),"0.0"),"%")</f>
@@ -35763,9 +36321,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A28" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="B28" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F24,1),"0.0"),"%")</f>
@@ -35781,9 +36338,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A29" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="B29" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F25,1),"0.0"),"%")</f>
@@ -35799,9 +36355,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A30" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="B30" s="25" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([2]output_table!F26,1),"0.0"),"%")</f>
@@ -35818,7 +36373,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -35841,7 +36396,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35898,9 +36453,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A7" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="B7" s="17" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F2,1),"0.0"),"%")</f>
@@ -35928,9 +36482,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A8" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="B8" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F3,1),"0.0"),"%")</f>
@@ -35958,9 +36511,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A9" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="B9" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F4,1),"0.0"),"%")</f>
@@ -35988,9 +36540,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A10" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="B10" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F5,1),"0.0"),"%")</f>
@@ -36018,9 +36569,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A11" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="B11" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F6,1),"0.0"),"%")</f>
@@ -36048,9 +36598,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A12" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="B12" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F7,1),"0.0"),"%")</f>
@@ -36078,9 +36627,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A13" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="B13" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F8,1),"0.0"),"%")</f>
@@ -36108,9 +36656,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A14" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="B14" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F9,1),"0.0"),"%")</f>
@@ -36138,9 +36685,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A15" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="B15" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F10,1),"0.0"),"%")</f>
@@ -36168,9 +36714,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A16" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="B16" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F11,1),"0.0"),"%")</f>
@@ -36198,9 +36743,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A17" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="B17" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F12,1),"0.0"),"%")</f>
@@ -36228,9 +36772,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A18" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="B18" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F13,1),"0.0"),"%")</f>
@@ -36258,9 +36801,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A19" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="B19" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F14,1),"0.0"),"%")</f>
@@ -36288,9 +36830,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A20" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="B20" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F15,1),"0.0"),"%")</f>
@@ -36318,9 +36859,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A21" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B21" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F16,1),"0.0"),"%")</f>
@@ -36348,9 +36888,8 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A22" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="B22" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F17,1),"0.0"),"%")</f>
@@ -36378,9 +36917,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A23" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="B23" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F18,1),"0.0"),"%")</f>
@@ -36408,9 +36946,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A24" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="B24" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F19,1),"0.0"),"%")</f>
@@ -36438,9 +36975,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A25" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="B25" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F20,1),"0.0"),"%")</f>
@@ -36468,9 +37004,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A26" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="B26" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F21,1),"0.0"),"%")</f>
@@ -36498,9 +37033,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A27" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="B27" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F22,1),"0.0"),"%")</f>
@@ -36528,9 +37062,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A28" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="B28" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F23,1),"0.0"),"%")</f>
@@ -36558,9 +37091,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A29" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="B29" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F24,1),"0.0"),"%")</f>
@@ -36588,9 +37120,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A30" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="B30" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F25,1),"0.0"),"%")</f>
@@ -36618,9 +37149,8 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A31" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="B31" s="25" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([3]output_table!F26,1),"0.0"),"%")</f>
@@ -36649,7 +37179,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -36676,7 +37206,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36710,9 +37240,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A6" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="B6" s="17" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F2,1),"0.0"),"%")</f>
@@ -36728,9 +37257,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A7" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="B7" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F3,1),"0.0"),"%")</f>
@@ -36746,9 +37274,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A8" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="B8" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F4,1),"0.0"),"%")</f>
@@ -36764,9 +37291,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A9" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="B9" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F5,1),"0.0"),"%")</f>
@@ -36782,9 +37308,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A10" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="B10" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F6,1),"0.0"),"%")</f>
@@ -36800,9 +37325,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A11" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="B11" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F7,1),"0.0"),"%")</f>
@@ -36818,9 +37342,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A12" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="B12" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F8,1),"0.0"),"%")</f>
@@ -36836,9 +37359,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A13" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="B13" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F9,1),"0.0"),"%")</f>
@@ -36854,9 +37376,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A14" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="B14" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F10,1),"0.0"),"%")</f>
@@ -36872,9 +37393,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A15" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="B15" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F11,1),"0.0"),"%")</f>
@@ -36890,9 +37410,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A16" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="B16" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F12,1),"0.0"),"%")</f>
@@ -36908,9 +37427,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A17" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="B17" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F13,1),"0.0"),"%")</f>
@@ -36926,9 +37444,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A18" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="B18" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F14,1),"0.0"),"%")</f>
@@ -36944,9 +37461,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A19" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="B19" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F15,1),"0.0"),"%")</f>
@@ -36962,9 +37478,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A20" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B20" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F16,1),"0.0"),"%")</f>
@@ -36980,9 +37495,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A21" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="B21" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F17,1),"0.0"),"%")</f>
@@ -36998,9 +37512,8 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A22" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="B22" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F18,1),"0.0"),"%")</f>
@@ -37016,9 +37529,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A23" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="B23" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F19,1),"0.0"),"%")</f>
@@ -37034,9 +37546,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A24" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="B24" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F20,1),"0.0"),"%")</f>
@@ -37052,9 +37563,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A25" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="B25" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F21,1),"0.0"),"%")</f>
@@ -37070,9 +37580,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A26" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="B26" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F22,1),"0.0"),"%")</f>
@@ -37088,9 +37597,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A27" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="B27" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F23,1),"0.0"),"%")</f>
@@ -37106,9 +37614,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A28" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="B28" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F24,1),"0.0"),"%")</f>
@@ -37124,9 +37631,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A29" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="B29" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F25,1),"0.0"),"%")</f>
@@ -37142,9 +37648,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A30" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="B30" s="25" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([5]output_table!F26,1),"0.0"),"%")</f>
@@ -37161,7 +37666,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -37183,8 +37688,8 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37256,13 +37761,21 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
+      <c r="A7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="17" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F2,1),"0.0"),"%")</f>
+        <v>1.5%</v>
+      </c>
+      <c r="C7" s="18" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G2,1),"0.0"),"%")</f>
+        <v>-2.7%</v>
+      </c>
+      <c r="D7" s="19" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H2,1),"0.0"),"%")</f>
+        <v>4.3%</v>
+      </c>
       <c r="E7" s="17" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F2,1),"0.0"),"%")</f>
         <v>1.4%</v>
@@ -37275,18 +37788,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H2,1),"0.0"),"%")</f>
         <v>4.1%</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="19"/>
+      <c r="H7" s="17" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F2,1),"0.0"),"%")</f>
+        <v>1.2%</v>
+      </c>
+      <c r="I7" s="18" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G2,1),"0.0"),"%")</f>
+        <v>-2.8%</v>
+      </c>
+      <c r="J7" s="19" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H2,1),"0.0"),"%")</f>
+        <v>4.0%</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
+      <c r="A8" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F3,1),"0.0"),"%")</f>
+        <v>-38.5%</v>
+      </c>
+      <c r="C8" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G3,1),"0.0"),"%")</f>
+        <v>-63.1%</v>
+      </c>
+      <c r="D8" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H3,1),"0.0"),"%")</f>
+        <v>24.6%</v>
+      </c>
       <c r="E8" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F3,1),"0.0"),"%")</f>
         <v>-37.8%</v>
@@ -37299,18 +37829,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H3,1),"0.0"),"%")</f>
         <v>25.9%</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
+      <c r="H8" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F3,1),"0.0"),"%")</f>
+        <v>-37.4%</v>
+      </c>
+      <c r="I8" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G3,1),"0.0"),"%")</f>
+        <v>-63.7%</v>
+      </c>
+      <c r="J8" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H3,1),"0.0"),"%")</f>
+        <v>26.3%</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
+      <c r="A9" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F4,1),"0.0"),"%")</f>
+        <v>-50.4%</v>
+      </c>
+      <c r="C9" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G4,1),"0.0"),"%")</f>
+        <v>-115.0%</v>
+      </c>
+      <c r="D9" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H4,1),"0.0"),"%")</f>
+        <v>64.5%</v>
+      </c>
       <c r="E9" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F4,1),"0.0"),"%")</f>
         <v>-50.5%</v>
@@ -37323,18 +37870,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H4,1),"0.0"),"%")</f>
         <v>64.8%</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
+      <c r="H9" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F4,1),"0.0"),"%")</f>
+        <v>-50.5%</v>
+      </c>
+      <c r="I9" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G4,1),"0.0"),"%")</f>
+        <v>-116.0%</v>
+      </c>
+      <c r="J9" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H4,1),"0.0"),"%")</f>
+        <v>65.4%</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
+      <c r="A10" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F5,1),"0.0"),"%")</f>
+        <v>-60.3%</v>
+      </c>
+      <c r="C10" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G5,1),"0.0"),"%")</f>
+        <v>-86.8%</v>
+      </c>
+      <c r="D10" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H5,1),"0.0"),"%")</f>
+        <v>26.5%</v>
+      </c>
       <c r="E10" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F5,1),"0.0"),"%")</f>
         <v>-60.5%</v>
@@ -37347,18 +37911,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H5,1),"0.0"),"%")</f>
         <v>26.2%</v>
       </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
+      <c r="H10" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F5,1),"0.0"),"%")</f>
+        <v>-60.9%</v>
+      </c>
+      <c r="I10" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G5,1),"0.0"),"%")</f>
+        <v>-86.3%</v>
+      </c>
+      <c r="J10" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H5,1),"0.0"),"%")</f>
+        <v>25.5%</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
+      <c r="A11" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F6,1),"0.0"),"%")</f>
+        <v>1.5%</v>
+      </c>
+      <c r="C11" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G6,1),"0.0"),"%")</f>
+        <v>0.4%</v>
+      </c>
+      <c r="D11" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H6,1),"0.0"),"%")</f>
+        <v>1.1%</v>
+      </c>
       <c r="E11" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F6,1),"0.0"),"%")</f>
         <v>1.5%</v>
@@ -37371,18 +37952,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H6,1),"0.0"),"%")</f>
         <v>1.1%</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
+      <c r="H11" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F6,1),"0.0"),"%")</f>
+        <v>1.5%</v>
+      </c>
+      <c r="I11" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G6,1),"0.0"),"%")</f>
+        <v>0.4%</v>
+      </c>
+      <c r="J11" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H6,1),"0.0"),"%")</f>
+        <v>1.2%</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F7,1),"0.0"),"%")</f>
+        <v>-21.2%</v>
+      </c>
+      <c r="C12" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G7,1),"0.0"),"%")</f>
+        <v>-30.0%</v>
+      </c>
+      <c r="D12" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H7,1),"0.0"),"%")</f>
+        <v>8.8%</v>
+      </c>
       <c r="E12" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F7,1),"0.0"),"%")</f>
         <v>-21.3%</v>
@@ -37395,18 +37993,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H7,1),"0.0"),"%")</f>
         <v>8.5%</v>
       </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="23"/>
+      <c r="H12" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F7,1),"0.0"),"%")</f>
+        <v>-21.3%</v>
+      </c>
+      <c r="I12" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G7,1),"0.0"),"%")</f>
+        <v>-29.6%</v>
+      </c>
+      <c r="J12" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H7,1),"0.0"),"%")</f>
+        <v>8.3%</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
+      <c r="A13" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F8,1),"0.0"),"%")</f>
+        <v>-64.0%</v>
+      </c>
+      <c r="C13" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G8,1),"0.0"),"%")</f>
+        <v>-47.7%</v>
+      </c>
+      <c r="D13" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H8,1),"0.0"),"%")</f>
+        <v>-16.3%</v>
+      </c>
       <c r="E13" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F8,1),"0.0"),"%")</f>
         <v>-64.1%</v>
@@ -37419,18 +38034,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H8,1),"0.0"),"%")</f>
         <v>-16.1%</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
+      <c r="H13" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F8,1),"0.0"),"%")</f>
+        <v>-64.2%</v>
+      </c>
+      <c r="I13" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G8,1),"0.0"),"%")</f>
+        <v>-48.2%</v>
+      </c>
+      <c r="J13" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H8,1),"0.0"),"%")</f>
+        <v>-16.0%</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
+      <c r="A14" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F9,1),"0.0"),"%")</f>
+        <v>-24.9%</v>
+      </c>
+      <c r="C14" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G9,1),"0.0"),"%")</f>
+        <v>-60.6%</v>
+      </c>
+      <c r="D14" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H9,1),"0.0"),"%")</f>
+        <v>35.7%</v>
+      </c>
       <c r="E14" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F9,1),"0.0"),"%")</f>
         <v>-24.9%</v>
@@ -37443,18 +38075,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H9,1),"0.0"),"%")</f>
         <v>35.9%</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
+      <c r="H14" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F9,1),"0.0"),"%")</f>
+        <v>-24.9%</v>
+      </c>
+      <c r="I14" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G9,1),"0.0"),"%")</f>
+        <v>-61.2%</v>
+      </c>
+      <c r="J14" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H9,1),"0.0"),"%")</f>
+        <v>36.3%</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
+      <c r="A15" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F10,1),"0.0"),"%")</f>
+        <v>-15.8%</v>
+      </c>
+      <c r="C15" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G10,1),"0.0"),"%")</f>
+        <v>6.4%</v>
+      </c>
+      <c r="D15" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H10,1),"0.0"),"%")</f>
+        <v>-22.2%</v>
+      </c>
       <c r="E15" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F10,1),"0.0"),"%")</f>
         <v>-15.7%</v>
@@ -37467,18 +38116,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H10,1),"0.0"),"%")</f>
         <v>-22.3%</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
+      <c r="H15" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F10,1),"0.0"),"%")</f>
+        <v>-15.6%</v>
+      </c>
+      <c r="I15" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G10,1),"0.0"),"%")</f>
+        <v>6.8%</v>
+      </c>
+      <c r="J15" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H10,1),"0.0"),"%")</f>
+        <v>-22.4%</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
+      <c r="A16" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F11,1),"0.0"),"%")</f>
+        <v>-27.8%</v>
+      </c>
+      <c r="C16" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G11,1),"0.0"),"%")</f>
+        <v>-28.2%</v>
+      </c>
+      <c r="D16" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H11,1),"0.0"),"%")</f>
+        <v>0.4%</v>
+      </c>
       <c r="E16" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F11,1),"0.0"),"%")</f>
         <v>-27.8%</v>
@@ -37491,18 +38157,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H11,1),"0.0"),"%")</f>
         <v>0.4%</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="23"/>
+      <c r="H16" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F11,1),"0.0"),"%")</f>
+        <v>-27.9%</v>
+      </c>
+      <c r="I16" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G11,1),"0.0"),"%")</f>
+        <v>-28.2%</v>
+      </c>
+      <c r="J16" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H11,1),"0.0"),"%")</f>
+        <v>0.3%</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
+      <c r="A17" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F12,1),"0.0"),"%")</f>
+        <v>-6.1%</v>
+      </c>
+      <c r="C17" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G12,1),"0.0"),"%")</f>
+        <v>-9.8%</v>
+      </c>
+      <c r="D17" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H12,1),"0.0"),"%")</f>
+        <v>3.8%</v>
+      </c>
       <c r="E17" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F12,1),"0.0"),"%")</f>
         <v>-5.7%</v>
@@ -37515,18 +38198,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H12,1),"0.0"),"%")</f>
         <v>4.4%</v>
       </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="23"/>
+      <c r="H17" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F12,1),"0.0"),"%")</f>
+        <v>-5.5%</v>
+      </c>
+      <c r="I17" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G12,1),"0.0"),"%")</f>
+        <v>-10.8%</v>
+      </c>
+      <c r="J17" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H12,1),"0.0"),"%")</f>
+        <v>5.3%</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
+      <c r="A18" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F13,1),"0.0"),"%")</f>
+        <v>-11.2%</v>
+      </c>
+      <c r="C18" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G13,1),"0.0"),"%")</f>
+        <v>-9.9%</v>
+      </c>
+      <c r="D18" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H13,1),"0.0"),"%")</f>
+        <v>-1.3%</v>
+      </c>
       <c r="E18" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F13,1),"0.0"),"%")</f>
         <v>-11.2%</v>
@@ -37539,18 +38239,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H13,1),"0.0"),"%")</f>
         <v>-1.3%</v>
       </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
+      <c r="H18" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F13,1),"0.0"),"%")</f>
+        <v>-11.2%</v>
+      </c>
+      <c r="I18" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G13,1),"0.0"),"%")</f>
+        <v>-9.9%</v>
+      </c>
+      <c r="J18" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H13,1),"0.0"),"%")</f>
+        <v>-1.3%</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
+      <c r="A19" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F14,1),"0.0"),"%")</f>
+        <v>-60.2%</v>
+      </c>
+      <c r="C19" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G14,1),"0.0"),"%")</f>
+        <v>-65.6%</v>
+      </c>
+      <c r="D19" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H14,1),"0.0"),"%")</f>
+        <v>5.4%</v>
+      </c>
       <c r="E19" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F14,1),"0.0"),"%")</f>
         <v>-60.1%</v>
@@ -37563,18 +38280,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H14,1),"0.0"),"%")</f>
         <v>6.0%</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
+      <c r="H19" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F14,1),"0.0"),"%")</f>
+        <v>-59.8%</v>
+      </c>
+      <c r="I19" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G14,1),"0.0"),"%")</f>
+        <v>-67.2%</v>
+      </c>
+      <c r="J19" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H14,1),"0.0"),"%")</f>
+        <v>7.4%</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
+      <c r="A20" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F15,1),"0.0"),"%")</f>
+        <v>-14.4%</v>
+      </c>
+      <c r="C20" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G15,1),"0.0"),"%")</f>
+        <v>4.7%</v>
+      </c>
+      <c r="D20" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H15,1),"0.0"),"%")</f>
+        <v>-19.1%</v>
+      </c>
       <c r="E20" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F15,1),"0.0"),"%")</f>
         <v>-14.3%</v>
@@ -37587,18 +38321,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H15,1),"0.0"),"%")</f>
         <v>-19.3%</v>
       </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
+      <c r="H20" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F15,1),"0.0"),"%")</f>
+        <v>-14.2%</v>
+      </c>
+      <c r="I20" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G15,1),"0.0"),"%")</f>
+        <v>5.2%</v>
+      </c>
+      <c r="J20" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H15,1),"0.0"),"%")</f>
+        <v>-19.4%</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
+      <c r="A21" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F16,1),"0.0"),"%")</f>
+        <v>-0.8%</v>
+      </c>
+      <c r="C21" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G16,1),"0.0"),"%")</f>
+        <v>1.8%</v>
+      </c>
+      <c r="D21" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H16,1),"0.0"),"%")</f>
+        <v>-2.7%</v>
+      </c>
       <c r="E21" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F16,1),"0.0"),"%")</f>
         <v>-0.9%</v>
@@ -37611,18 +38362,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H16,1),"0.0"),"%")</f>
         <v>-2.7%</v>
       </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="23"/>
+      <c r="H21" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F16,1),"0.0"),"%")</f>
+        <v>-0.9%</v>
+      </c>
+      <c r="I21" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G16,1),"0.0"),"%")</f>
+        <v>1.9%</v>
+      </c>
+      <c r="J21" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H16,1),"0.0"),"%")</f>
+        <v>-2.9%</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
+      <c r="A22" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F17,1),"0.0"),"%")</f>
+        <v>-52.0%</v>
+      </c>
+      <c r="C22" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G17,1),"0.0"),"%")</f>
+        <v>-95.1%</v>
+      </c>
+      <c r="D22" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H17,1),"0.0"),"%")</f>
+        <v>43.1%</v>
+      </c>
       <c r="E22" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F17,1),"0.0"),"%")</f>
         <v>-52.1%</v>
@@ -37635,18 +38403,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H17,1),"0.0"),"%")</f>
         <v>42.5%</v>
       </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
+      <c r="H22" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F17,1),"0.0"),"%")</f>
+        <v>-52.1%</v>
+      </c>
+      <c r="I22" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G17,1),"0.0"),"%")</f>
+        <v>-93.8%</v>
+      </c>
+      <c r="J22" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H17,1),"0.0"),"%")</f>
+        <v>41.7%</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
+      <c r="A23" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F18,1),"0.0"),"%")</f>
+        <v>-46.6%</v>
+      </c>
+      <c r="C23" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G18,1),"0.0"),"%")</f>
+        <v>-139.5%</v>
+      </c>
+      <c r="D23" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H18,1),"0.0"),"%")</f>
+        <v>92.8%</v>
+      </c>
       <c r="E23" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F18,1),"0.0"),"%")</f>
         <v>-46.8%</v>
@@ -37659,18 +38444,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H18,1),"0.0"),"%")</f>
         <v>93.5%</v>
       </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
+      <c r="H23" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F18,1),"0.0"),"%")</f>
+        <v>-47.2%</v>
+      </c>
+      <c r="I23" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G18,1),"0.0"),"%")</f>
+        <v>-141.8%</v>
+      </c>
+      <c r="J23" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H18,1),"0.0"),"%")</f>
+        <v>94.6%</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
+      <c r="A24" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F19,1),"0.0"),"%")</f>
+        <v>-30.7%</v>
+      </c>
+      <c r="C24" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G19,1),"0.0"),"%")</f>
+        <v>-77.2%</v>
+      </c>
+      <c r="D24" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H19,1),"0.0"),"%")</f>
+        <v>46.6%</v>
+      </c>
       <c r="E24" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F19,1),"0.0"),"%")</f>
         <v>-30.5%</v>
@@ -37683,18 +38485,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H19,1),"0.0"),"%")</f>
         <v>46.7%</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="23"/>
+      <c r="H24" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F19,1),"0.0"),"%")</f>
+        <v>-30.2%</v>
+      </c>
+      <c r="I24" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G19,1),"0.0"),"%")</f>
+        <v>-77.2%</v>
+      </c>
+      <c r="J24" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H19,1),"0.0"),"%")</f>
+        <v>47.0%</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="23"/>
+      <c r="A25" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F20,1),"0.0"),"%")</f>
+        <v>2.7%</v>
+      </c>
+      <c r="C25" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G20,1),"0.0"),"%")</f>
+        <v>-35.3%</v>
+      </c>
+      <c r="D25" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H20,1),"0.0"),"%")</f>
+        <v>38.0%</v>
+      </c>
       <c r="E25" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F20,1),"0.0"),"%")</f>
         <v>2.2%</v>
@@ -37707,18 +38526,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H20,1),"0.0"),"%")</f>
         <v>37.7%</v>
       </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="23"/>
+      <c r="H25" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F20,1),"0.0"),"%")</f>
+        <v>1.7%</v>
+      </c>
+      <c r="I25" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G20,1),"0.0"),"%")</f>
+        <v>-35.6%</v>
+      </c>
+      <c r="J25" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H20,1),"0.0"),"%")</f>
+        <v>37.3%</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
+      <c r="A26" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F21,1),"0.0"),"%")</f>
+        <v>0.6%</v>
+      </c>
+      <c r="C26" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G21,1),"0.0"),"%")</f>
+        <v>-2.5%</v>
+      </c>
+      <c r="D26" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H21,1),"0.0"),"%")</f>
+        <v>3.2%</v>
+      </c>
       <c r="E26" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F21,1),"0.0"),"%")</f>
         <v>0.7%</v>
@@ -37731,18 +38567,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H21,1),"0.0"),"%")</f>
         <v>3.2%</v>
       </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="23"/>
+      <c r="H26" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F21,1),"0.0"),"%")</f>
+        <v>0.7%</v>
+      </c>
+      <c r="I26" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G21,1),"0.0"),"%")</f>
+        <v>-2.5%</v>
+      </c>
+      <c r="J26" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H21,1),"0.0"),"%")</f>
+        <v>3.2%</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
+      <c r="A27" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F22,1),"0.0"),"%")</f>
+        <v>-8.5%</v>
+      </c>
+      <c r="C27" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G22,1),"0.0"),"%")</f>
+        <v>-19.1%</v>
+      </c>
+      <c r="D27" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H22,1),"0.0"),"%")</f>
+        <v>10.6%</v>
+      </c>
       <c r="E27" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F22,1),"0.0"),"%")</f>
         <v>-8.7%</v>
@@ -37755,18 +38608,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H22,1),"0.0"),"%")</f>
         <v>10.8%</v>
       </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="23"/>
+      <c r="H27" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F22,1),"0.0"),"%")</f>
+        <v>-8.9%</v>
+      </c>
+      <c r="I27" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G22,1),"0.0"),"%")</f>
+        <v>-19.9%</v>
+      </c>
+      <c r="J27" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H22,1),"0.0"),"%")</f>
+        <v>11.0%</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
+      <c r="A28" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F23,1),"0.0"),"%")</f>
+        <v>-54.4%</v>
+      </c>
+      <c r="C28" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G23,1),"0.0"),"%")</f>
+        <v>-26.3%</v>
+      </c>
+      <c r="D28" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H23,1),"0.0"),"%")</f>
+        <v>-28.1%</v>
+      </c>
       <c r="E28" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F23,1),"0.0"),"%")</f>
         <v>-54.3%</v>
@@ -37779,18 +38649,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H23,1),"0.0"),"%")</f>
         <v>-28.0%</v>
       </c>
-      <c r="H28" s="21"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="23"/>
+      <c r="H28" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F23,1),"0.0"),"%")</f>
+        <v>-54.3%</v>
+      </c>
+      <c r="I28" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G23,1),"0.0"),"%")</f>
+        <v>-26.5%</v>
+      </c>
+      <c r="J28" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H23,1),"0.0"),"%")</f>
+        <v>-27.8%</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
+      <c r="A29" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F24,1),"0.0"),"%")</f>
+        <v>-35.1%</v>
+      </c>
+      <c r="C29" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G24,1),"0.0"),"%")</f>
+        <v>-38.0%</v>
+      </c>
+      <c r="D29" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H24,1),"0.0"),"%")</f>
+        <v>2.9%</v>
+      </c>
       <c r="E29" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F24,1),"0.0"),"%")</f>
         <v>-35.3%</v>
@@ -37803,18 +38690,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H24,1),"0.0"),"%")</f>
         <v>2.7%</v>
       </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="23"/>
+      <c r="H29" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F24,1),"0.0"),"%")</f>
+        <v>-35.6%</v>
+      </c>
+      <c r="I29" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G24,1),"0.0"),"%")</f>
+        <v>-38.2%</v>
+      </c>
+      <c r="J29" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H24,1),"0.0"),"%")</f>
+        <v>2.6%</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="23"/>
+      <c r="A30" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F25,1),"0.0"),"%")</f>
+        <v>-43.9%</v>
+      </c>
+      <c r="C30" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G25,1),"0.0"),"%")</f>
+        <v>-27.4%</v>
+      </c>
+      <c r="D30" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H25,1),"0.0"),"%")</f>
+        <v>-16.5%</v>
+      </c>
       <c r="E30" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F25,1),"0.0"),"%")</f>
         <v>-44.0%</v>
@@ -37827,18 +38731,35 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H25,1),"0.0"),"%")</f>
         <v>-16.8%</v>
       </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="23"/>
+      <c r="H30" s="21" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F25,1),"0.0"),"%")</f>
+        <v>-44.2%</v>
+      </c>
+      <c r="I30" s="22" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G25,1),"0.0"),"%")</f>
+        <v>-26.9%</v>
+      </c>
+      <c r="J30" s="23" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H25,1),"0.0"),"%")</f>
+        <v>-17.2%</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="27"/>
+      <c r="A31" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="25" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!F26,1),"0.0"),"%")</f>
+        <v>-0.4%</v>
+      </c>
+      <c r="C31" s="26" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!G26,1),"0.0"),"%")</f>
+        <v>2.5%</v>
+      </c>
+      <c r="D31" s="27" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([14]output_table!H26,1),"0.0"),"%")</f>
+        <v>-3.0%</v>
+      </c>
       <c r="E31" s="25" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!F26,1),"0.0"),"%")</f>
         <v>-0.4%</v>
@@ -37851,13 +38772,22 @@
         <f aca="false">CONCATENATE(TEXT(ROUND([6]output_table!H26,1),"0.0"),"%")</f>
         <v>-3.0%</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
+      <c r="H31" s="25" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!F26,1),"0.0"),"%")</f>
+        <v>-0.4%</v>
+      </c>
+      <c r="I31" s="26" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!G26,1),"0.0"),"%")</f>
+        <v>2.7%</v>
+      </c>
+      <c r="J31" s="27" t="str">
+        <f aca="false">CONCATENATE(TEXT(ROUND([15]output_table!H26,1),"0.0"),"%")</f>
+        <v>-3.2%</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -37885,7 +38815,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37942,9 +38872,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A7" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="B7" s="17" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F2,1),"0.0"),"%")</f>
@@ -37972,9 +38901,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A8" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="B8" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F3,1),"0.0"),"%")</f>
@@ -38002,9 +38930,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A9" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="B9" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F4,1),"0.0"),"%")</f>
@@ -38032,9 +38959,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A10" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="B10" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F5,1),"0.0"),"%")</f>
@@ -38062,9 +38988,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A11" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="B11" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F6,1),"0.0"),"%")</f>
@@ -38092,9 +39017,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A12" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="B12" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F7,1),"0.0"),"%")</f>
@@ -38122,9 +39046,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A13" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="B13" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F8,1),"0.0"),"%")</f>
@@ -38152,9 +39075,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A14" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="B14" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F9,1),"0.0"),"%")</f>
@@ -38182,9 +39104,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A15" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="B15" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F10,1),"0.0"),"%")</f>
@@ -38212,9 +39133,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A16" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="B16" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F11,1),"0.0"),"%")</f>
@@ -38242,9 +39162,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A17" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="B17" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F12,1),"0.0"),"%")</f>
@@ -38272,9 +39191,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A18" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="B18" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F13,1),"0.0"),"%")</f>
@@ -38302,9 +39220,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A19" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="B19" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F14,1),"0.0"),"%")</f>
@@ -38332,9 +39249,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A20" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="B20" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F15,1),"0.0"),"%")</f>
@@ -38362,9 +39278,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A21" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B21" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F16,1),"0.0"),"%")</f>
@@ -38392,9 +39307,8 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A22" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="B22" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F17,1),"0.0"),"%")</f>
@@ -38422,9 +39336,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A23" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="B23" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F18,1),"0.0"),"%")</f>
@@ -38452,9 +39365,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A24" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="B24" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F19,1),"0.0"),"%")</f>
@@ -38482,9 +39394,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A25" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="B25" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F20,1),"0.0"),"%")</f>
@@ -38512,9 +39423,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A26" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="B26" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F21,1),"0.0"),"%")</f>
@@ -38542,9 +39452,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A27" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="B27" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F22,1),"0.0"),"%")</f>
@@ -38572,9 +39481,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A28" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="B28" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F23,1),"0.0"),"%")</f>
@@ -38602,9 +39510,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A29" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="B29" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F24,1),"0.0"),"%")</f>
@@ -38632,9 +39539,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A30" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="B30" s="21" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F25,1),"0.0"),"%")</f>
@@ -38662,9 +39568,8 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="A31" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="B31" s="25" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([7]output_table!F26,1),"0.0"),"%")</f>
@@ -38693,7 +39598,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -38755,7 +39660,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="B6" s="30" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([9]volatility_by_decade!B2,1),"0.0"),"%")</f>
@@ -38772,7 +39677,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B7" s="34" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([9]volatility_by_decade!B3,1),"0.0"),"%")</f>
@@ -38789,7 +39694,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="B8" s="34" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([9]volatility_by_decade!B4,1),"0.0"),"%")</f>
@@ -38806,7 +39711,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B9" s="38" t="str">
         <f aca="false">CONCATENATE(TEXT(ROUND([9]volatility_by_decade!B5,1),"0.0"),"%")</f>
@@ -38828,7 +39733,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>

</xml_diff>

<commit_message>
Volatility tables with sigma = 0.5 and 1.3
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -632,7 +632,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -689,8 +689,15 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCE181E"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -701,6 +708,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -843,7 +856,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -988,6 +1001,14 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1045,10 +1066,10 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -1104,7 +1125,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1114,277 +1135,277 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="F2">
-            <v>-0.871995016938059</v>
+            <v>-10.5774800004832</v>
           </cell>
           <cell r="G2">
-            <v>-4.78527761838807</v>
+            <v>11.9157011202646</v>
           </cell>
           <cell r="H2">
-            <v>3.91328260145002</v>
+            <v>-22.4931811207477</v>
           </cell>
         </row>
         <row r="3">
           <cell r="F3">
-            <v>-24.4374821423859</v>
+            <v>-50.2702420863422</v>
           </cell>
           <cell r="G3">
-            <v>-54.3372392480144</v>
+            <v>-58.8402847932354</v>
           </cell>
           <cell r="H3">
-            <v>29.8997571056286</v>
+            <v>8.57004270689324</v>
           </cell>
         </row>
         <row r="4">
           <cell r="F4">
-            <v>-51.9067343614722</v>
+            <v>-75.4604247091419</v>
           </cell>
           <cell r="G4">
-            <v>-120.014431542971</v>
+            <v>-32.7713766296395</v>
           </cell>
           <cell r="H4">
-            <v>68.1076971814993</v>
+            <v>-42.6890480795024</v>
           </cell>
         </row>
         <row r="5">
           <cell r="F5">
-            <v>-58.0690718007581</v>
+            <v>-76.9039646345329</v>
           </cell>
           <cell r="G5">
-            <v>-79.9086805784265</v>
+            <v>-54.9844897443001</v>
           </cell>
           <cell r="H5">
-            <v>21.8396087776684</v>
+            <v>-21.9194748902328</v>
           </cell>
         </row>
         <row r="6">
           <cell r="F6">
-            <v>0.148798216700991</v>
+            <v>1.82813106553456</v>
           </cell>
           <cell r="G6">
-            <v>-0.517503332565823</v>
+            <v>-6.84938272436293</v>
           </cell>
           <cell r="H6">
-            <v>0.666301549266814</v>
+            <v>8.67751378989749</v>
           </cell>
         </row>
         <row r="7">
           <cell r="F7">
-            <v>-14.2564850715132</v>
+            <v>-56.6601441804896</v>
           </cell>
           <cell r="G7">
-            <v>-53.0229168922839</v>
+            <v>-190.321986540188</v>
           </cell>
           <cell r="H7">
-            <v>38.7664318207707</v>
+            <v>133.661842359698</v>
           </cell>
         </row>
         <row r="8">
           <cell r="F8">
-            <v>-49.2452883411108</v>
+            <v>-80.0138856686181</v>
           </cell>
           <cell r="G8">
-            <v>-37.966738886339</v>
+            <v>-11.8707034251192</v>
           </cell>
           <cell r="H8">
-            <v>-11.2785494547718</v>
+            <v>-68.1431822434988</v>
           </cell>
         </row>
         <row r="9">
           <cell r="F9">
-            <v>-27.7226086616764</v>
+            <v>-41.6616411332547</v>
           </cell>
           <cell r="G9">
-            <v>-54.5526515343252</v>
+            <v>-23.4405608368549</v>
           </cell>
           <cell r="H9">
-            <v>26.8300428726488</v>
+            <v>-18.2210802963999</v>
           </cell>
         </row>
         <row r="10">
           <cell r="F10">
-            <v>-11.3835253898429</v>
+            <v>-27.6058793004082</v>
           </cell>
           <cell r="G10">
-            <v>4.10072534058516</v>
+            <v>56.1379934275976</v>
           </cell>
           <cell r="H10">
-            <v>-15.484250730428</v>
+            <v>-83.7438727280057</v>
           </cell>
         </row>
         <row r="11">
           <cell r="F11">
-            <v>-19.3471852953465</v>
+            <v>-52.7757329740792</v>
           </cell>
           <cell r="G11">
-            <v>-25.5467838279911</v>
+            <v>-5.18258098908403</v>
           </cell>
           <cell r="H11">
-            <v>6.19959853264459</v>
+            <v>-47.5931519849952</v>
           </cell>
         </row>
         <row r="12">
           <cell r="F12">
-            <v>-19.6861749866989</v>
+            <v>-42.1403214905773</v>
           </cell>
           <cell r="G12">
-            <v>-2.33002931491005</v>
+            <v>69.9629814316786</v>
           </cell>
           <cell r="H12">
-            <v>-17.3561456717888</v>
+            <v>-112.103302922256</v>
           </cell>
         </row>
         <row r="13">
           <cell r="F13">
-            <v>-17.4660605201418</v>
+            <v>-39.0602773113667</v>
           </cell>
           <cell r="G13">
-            <v>-6.36371613876475</v>
+            <v>-18.4949753724605</v>
           </cell>
           <cell r="H13">
-            <v>-11.102344381377</v>
+            <v>-20.5653019389062</v>
           </cell>
         </row>
         <row r="14">
           <cell r="F14">
-            <v>-42.3678389613345</v>
+            <v>-60.3826540757764</v>
           </cell>
           <cell r="G14">
-            <v>-50.9302170187423</v>
+            <v>-22.6213245775179</v>
           </cell>
           <cell r="H14">
-            <v>8.56237805740784</v>
+            <v>-37.7613294982585</v>
           </cell>
         </row>
         <row r="15">
           <cell r="F15">
-            <v>-10.6176015864681</v>
+            <v>-31.1829960577724</v>
           </cell>
           <cell r="G15">
-            <v>3.04484286407378</v>
+            <v>55.3170195400885</v>
           </cell>
           <cell r="H15">
-            <v>-13.6624444505419</v>
+            <v>-86.5000155978609</v>
           </cell>
         </row>
         <row r="16">
           <cell r="F16">
-            <v>2.96940293156509</v>
+            <v>-2.39769981678716</v>
           </cell>
           <cell r="G16">
-            <v>0.754191321264443</v>
+            <v>16.4710157286001</v>
           </cell>
           <cell r="H16">
-            <v>2.21521161030064</v>
+            <v>-18.8687155453873</v>
           </cell>
         </row>
         <row r="17">
           <cell r="F17">
-            <v>-46.7974722117531</v>
+            <v>-71.4490451736532</v>
           </cell>
           <cell r="G17">
-            <v>-57.8010968696742</v>
+            <v>-27.5872663100018</v>
           </cell>
           <cell r="H17">
-            <v>11.0036246579211</v>
+            <v>-43.8617788636514</v>
           </cell>
         </row>
         <row r="18">
           <cell r="F18">
-            <v>-39.8552026477866</v>
+            <v>-77.7242558035879</v>
           </cell>
           <cell r="G18">
-            <v>-91.2143662445799</v>
+            <v>-37.9692833960334</v>
           </cell>
           <cell r="H18">
-            <v>51.3591635967933</v>
+            <v>-39.7549724075545</v>
           </cell>
         </row>
         <row r="19">
           <cell r="F19">
-            <v>-20.5316753152855</v>
+            <v>-32.8139110095778</v>
           </cell>
           <cell r="G19">
-            <v>-88.9409467706447</v>
+            <v>-54.693192934407</v>
           </cell>
           <cell r="H19">
-            <v>68.4092714553592</v>
+            <v>21.8792819248292</v>
           </cell>
         </row>
         <row r="20">
           <cell r="F20">
-            <v>-4.48722535326793</v>
+            <v>-20.1935445388272</v>
           </cell>
           <cell r="G20">
-            <v>-49.6369095325512</v>
+            <v>-7.0205522438127</v>
           </cell>
           <cell r="H20">
-            <v>45.1496841792833</v>
+            <v>-13.1729922950144</v>
           </cell>
         </row>
         <row r="21">
           <cell r="F21">
-            <v>2.42106592073112</v>
+            <v>4.05489812284114</v>
           </cell>
           <cell r="G21">
-            <v>-4.58193011121156</v>
+            <v>-5.7669814061569</v>
           </cell>
           <cell r="H21">
-            <v>7.00299603194268</v>
+            <v>9.82187952899806</v>
           </cell>
         </row>
         <row r="22">
           <cell r="F22">
-            <v>-1.45737451200485</v>
+            <v>1.24804916893947</v>
           </cell>
           <cell r="G22">
-            <v>-7.98375863200927</v>
+            <v>-1393.65629943119</v>
           </cell>
           <cell r="H22">
-            <v>6.52638412000442</v>
+            <v>1394.90434860013</v>
           </cell>
         </row>
         <row r="23">
           <cell r="F23">
-            <v>-38.0717854226395</v>
+            <v>-84.4632238182775</v>
           </cell>
           <cell r="G23">
-            <v>-24.5862184231078</v>
+            <v>-27.6165975484058</v>
           </cell>
           <cell r="H23">
-            <v>-13.4855669995317</v>
+            <v>-56.8466262698718</v>
           </cell>
         </row>
         <row r="24">
           <cell r="F24">
-            <v>-30.7753648851186</v>
+            <v>-48.2109191480942</v>
           </cell>
           <cell r="G24">
-            <v>-35.6293815819547</v>
+            <v>26.3421457661312</v>
           </cell>
           <cell r="H24">
-            <v>4.85401669683606</v>
+            <v>-74.5530649142253</v>
           </cell>
         </row>
         <row r="25">
           <cell r="F25">
-            <v>-28.2944435893703</v>
+            <v>-65.9916346739683</v>
           </cell>
           <cell r="G25">
-            <v>-20.9917282784647</v>
+            <v>9.14574639988598</v>
           </cell>
           <cell r="H25">
-            <v>-7.30271531090558</v>
+            <v>-75.1373810738542</v>
           </cell>
         </row>
         <row r="26">
           <cell r="F26">
-            <v>0.274887888504036</v>
+            <v>-1.3417262111894</v>
           </cell>
           <cell r="G26">
-            <v>0.483104676231486</v>
+            <v>14.9561161589925</v>
           </cell>
           <cell r="H26">
-            <v>-0.20821678772745</v>
+            <v>-16.2978423701819</v>
           </cell>
         </row>
       </sheetData>
@@ -1393,7 +1414,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1403,277 +1424,277 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="F2">
-            <v>-7.23492731217544</v>
+            <v>-0.803760370503652</v>
           </cell>
           <cell r="G2">
-            <v>23.7645038137774</v>
+            <v>-1.49140452596171</v>
           </cell>
           <cell r="H2">
-            <v>-30.9994311259528</v>
+            <v>0.68764415545807</v>
           </cell>
         </row>
         <row r="3">
           <cell r="F3">
-            <v>-22.8230753231275</v>
+            <v>-41.6684080682788</v>
           </cell>
           <cell r="G3">
-            <v>15.6385428602272</v>
+            <v>-80.6512346701537</v>
           </cell>
           <cell r="H3">
-            <v>-38.4616181833547</v>
+            <v>38.9828266018749</v>
           </cell>
         </row>
         <row r="4">
           <cell r="F4">
-            <v>-77.417062133289</v>
+            <v>-61.8351738247193</v>
           </cell>
           <cell r="G4">
-            <v>37.6039161400117</v>
+            <v>-68.5256528686372</v>
           </cell>
           <cell r="H4">
-            <v>-115.020978273301</v>
+            <v>6.69047904391785</v>
           </cell>
         </row>
         <row r="5">
           <cell r="F5">
-            <v>-81.3742436866602</v>
+            <v>-67.8704614714606</v>
           </cell>
           <cell r="G5">
-            <v>-114.810123085594</v>
+            <v>-75.5850938906485</v>
           </cell>
           <cell r="H5">
-            <v>33.4358793989334</v>
+            <v>7.71463241918783</v>
           </cell>
         </row>
         <row r="6">
           <cell r="F6">
-            <v>-0.227964164184585</v>
+            <v>0.761017944259593</v>
           </cell>
           <cell r="G6">
-            <v>1.88861176725159</v>
+            <v>0.151865848969158</v>
           </cell>
           <cell r="H6">
-            <v>-2.11657593143618</v>
+            <v>0.609152095290436</v>
           </cell>
         </row>
         <row r="7">
           <cell r="F7">
-            <v>-60.3481275834134</v>
+            <v>-32.2614192993616</v>
           </cell>
           <cell r="G7">
-            <v>-42.4098633842026</v>
+            <v>-33.4786565384342</v>
           </cell>
           <cell r="H7">
-            <v>-17.9382641992108</v>
+            <v>1.21723723907263</v>
           </cell>
         </row>
         <row r="8">
           <cell r="F8">
-            <v>-80.5623863063795</v>
+            <v>-73.9941720766543</v>
           </cell>
           <cell r="G8">
-            <v>22.2387408478649</v>
+            <v>-44.1657827097308</v>
           </cell>
           <cell r="H8">
-            <v>-102.801127154244</v>
+            <v>-29.8283893669235</v>
           </cell>
         </row>
         <row r="9">
           <cell r="F9">
-            <v>-10.2549710959205</v>
+            <v>-36.2862348876865</v>
           </cell>
           <cell r="G9">
-            <v>-2.19850232691694</v>
+            <v>-43.9959968702868</v>
           </cell>
           <cell r="H9">
-            <v>-8.05646876900356</v>
+            <v>7.70976198260029</v>
           </cell>
         </row>
         <row r="10">
           <cell r="F10">
-            <v>19.9010897848067</v>
+            <v>-19.5022920583921</v>
           </cell>
           <cell r="G10">
-            <v>83.7714983171599</v>
+            <v>22.9354732647409</v>
           </cell>
           <cell r="H10">
-            <v>-63.8704085323531</v>
+            <v>-42.437765323133</v>
           </cell>
         </row>
         <row r="11">
           <cell r="F11">
-            <v>157.632433295042</v>
+            <v>-50.2685713897412</v>
           </cell>
           <cell r="G11">
-            <v>47.9272941067823</v>
+            <v>-59.5439688399256</v>
           </cell>
           <cell r="H11">
-            <v>109.70513918826</v>
+            <v>9.2753974501844</v>
           </cell>
         </row>
         <row r="12">
           <cell r="F12">
-            <v>-15.8048493772097</v>
+            <v>-4.18007322504184</v>
           </cell>
           <cell r="G12">
-            <v>19.6454646122422</v>
+            <v>17.6776699242765</v>
           </cell>
           <cell r="H12">
-            <v>-35.4503139894519</v>
+            <v>-21.8577431493184</v>
           </cell>
         </row>
         <row r="13">
           <cell r="F13">
-            <v>-7.49476493598397</v>
+            <v>-6.22459164831054</v>
           </cell>
           <cell r="G13">
-            <v>-0.779280541311926</v>
+            <v>-2.02188255754279</v>
           </cell>
           <cell r="H13">
-            <v>-6.71548439467204</v>
+            <v>-4.20270909076775</v>
           </cell>
         </row>
         <row r="14">
           <cell r="F14">
-            <v>-31.5300992401331</v>
+            <v>-59.3220758737135</v>
           </cell>
           <cell r="G14">
-            <v>-23.7501064971338</v>
+            <v>-51.8659697057861</v>
           </cell>
           <cell r="H14">
-            <v>-7.77999274299929</v>
+            <v>-7.4561061679274</v>
           </cell>
         </row>
         <row r="15">
           <cell r="F15">
-            <v>-5.49753947063335</v>
+            <v>-21.1747256800595</v>
           </cell>
           <cell r="G15">
-            <v>65.937894183685</v>
+            <v>20.6559022504728</v>
           </cell>
           <cell r="H15">
-            <v>-71.4354336543184</v>
+            <v>-41.8306279305323</v>
           </cell>
         </row>
         <row r="16">
           <cell r="F16">
-            <v>7.9719948086892</v>
+            <v>-1.08342431981264</v>
           </cell>
           <cell r="G16">
-            <v>17.3708435483298</v>
+            <v>4.68465218392612</v>
           </cell>
           <cell r="H16">
-            <v>-9.39884873964065</v>
+            <v>-5.76807650373878</v>
           </cell>
         </row>
         <row r="17">
           <cell r="F17">
-            <v>-33.1043806473291</v>
+            <v>-45.5866497568974</v>
           </cell>
           <cell r="G17">
-            <v>-65.5061779791485</v>
+            <v>-48.8027441113953</v>
           </cell>
           <cell r="H17">
-            <v>32.4017973318194</v>
+            <v>3.21609435449784</v>
           </cell>
         </row>
         <row r="18">
           <cell r="F18">
-            <v>-34.7105652883372</v>
+            <v>-68.9380336386343</v>
           </cell>
           <cell r="G18">
-            <v>-18.8868133215729</v>
+            <v>-88.9750248849365</v>
           </cell>
           <cell r="H18">
-            <v>-15.8237519667643</v>
+            <v>20.0369912463023</v>
           </cell>
         </row>
         <row r="19">
           <cell r="F19">
-            <v>-38.2826257083383</v>
+            <v>-36.0600107403677</v>
           </cell>
           <cell r="G19">
-            <v>-37.7981614204648</v>
+            <v>-62.9796204238378</v>
           </cell>
           <cell r="H19">
-            <v>-0.484464287873454</v>
+            <v>26.9196096834701</v>
           </cell>
         </row>
         <row r="20">
           <cell r="F20">
-            <v>-5.82872078297532</v>
+            <v>-0.34493809491938</v>
           </cell>
           <cell r="G20">
-            <v>166.23371979197</v>
+            <v>-42.3712662360076</v>
           </cell>
           <cell r="H20">
-            <v>-172.062440574945</v>
+            <v>42.0263281410882</v>
           </cell>
         </row>
         <row r="21">
           <cell r="F21">
-            <v>2.64858142588495</v>
+            <v>-0.272427443717159</v>
           </cell>
           <cell r="G21">
-            <v>10.6312081109899</v>
+            <v>-3.47716281465467</v>
           </cell>
           <cell r="H21">
-            <v>-7.98262668510493</v>
+            <v>3.20473537093751</v>
           </cell>
         </row>
         <row r="22">
           <cell r="F22">
-            <v>79.2225852507143</v>
+            <v>0.624883185251995</v>
           </cell>
           <cell r="G22">
-            <v>80.7671138129608</v>
+            <v>-1.56291315252097</v>
           </cell>
           <cell r="H22">
-            <v>-1.54452856224645</v>
+            <v>2.18779633777296</v>
           </cell>
         </row>
         <row r="23">
           <cell r="F23">
-            <v>-53.3366574083791</v>
+            <v>-73.3969487507731</v>
           </cell>
           <cell r="G23">
-            <v>33.9166529569355</v>
+            <v>-47.9863715239884</v>
           </cell>
           <cell r="H23">
-            <v>-87.2533103653146</v>
+            <v>-25.4105772267847</v>
           </cell>
         </row>
         <row r="24">
           <cell r="F24">
-            <v>34.0016562998975</v>
+            <v>-38.1263086841299</v>
           </cell>
           <cell r="G24">
-            <v>46.5582311452327</v>
+            <v>-0.413882276424571</v>
           </cell>
           <cell r="H24">
-            <v>-12.5565748453352</v>
+            <v>-37.7124264077053</v>
           </cell>
         </row>
         <row r="25">
           <cell r="F25">
-            <v>-0.387560202024685</v>
+            <v>-53.6629909352087</v>
           </cell>
           <cell r="G25">
-            <v>114.323422022419</v>
+            <v>-27.9887122120898</v>
           </cell>
           <cell r="H25">
-            <v>-114.710982224443</v>
+            <v>-25.674278723119</v>
           </cell>
         </row>
         <row r="26">
           <cell r="F26">
-            <v>21.0206312128304</v>
+            <v>-0.550271986507331</v>
           </cell>
           <cell r="G26">
-            <v>35.9960903355552</v>
+            <v>0.487407204935892</v>
           </cell>
           <cell r="H26">
-            <v>-14.9754591227248</v>
+            <v>-1.03767919144322</v>
           </cell>
         </row>
       </sheetData>
@@ -30138,7 +30159,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30167,8 +30188,8 @@
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30" t="str">
-        <f aca="false">CONCATENATE(_xlfn.UNICHAR(963)," = 2")</f>
-        <v>σ = 2</v>
+        <f aca="false">CONCATENATE(_xlfn.UNICHAR(963)," = 1.3")</f>
+        <v>σ = 1.3</v>
       </c>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
@@ -30199,28 +30220,28 @@
         <v>91</v>
       </c>
       <c r="B7" s="17" t="n">
-        <f aca="false">[29]output_table!F2/100</f>
-        <v>-0.00871995016938059</v>
+        <f aca="false">[17]output_table!F2/100</f>
+        <v>-0.105774800004832</v>
       </c>
       <c r="C7" s="18" t="n">
-        <f aca="false">[29]output_table!G2/100</f>
-        <v>-0.0478527761838807</v>
+        <f aca="false">[17]output_table!G2/100</f>
+        <v>0.119157011202646</v>
       </c>
       <c r="D7" s="19" t="n">
-        <f aca="false">[29]output_table!H2/100</f>
-        <v>0.0391328260145002</v>
+        <f aca="false">[17]output_table!H2/100</f>
+        <v>-0.224931811207477</v>
       </c>
       <c r="E7" s="17" t="n">
-        <f aca="false">[30]output_table!F2/100</f>
-        <v>-0.0723492731217544</v>
+        <f aca="false">[18]output_table!F2/100</f>
+        <v>-0.00803760370503652</v>
       </c>
       <c r="F7" s="18" t="n">
-        <f aca="false">[30]output_table!G2/100</f>
-        <v>0.237645038137774</v>
+        <f aca="false">[18]output_table!G2/100</f>
+        <v>-0.0149140452596171</v>
       </c>
       <c r="G7" s="19" t="n">
-        <f aca="false">[30]output_table!H2/100</f>
-        <v>-0.309994311259528</v>
+        <f aca="false">[18]output_table!H2/100</f>
+        <v>0.0068764415545807</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30228,28 +30249,28 @@
         <v>92</v>
       </c>
       <c r="B8" s="21" t="n">
-        <f aca="false">[29]output_table!F3/100</f>
-        <v>-0.244374821423859</v>
+        <f aca="false">[17]output_table!F3/100</f>
+        <v>-0.502702420863422</v>
       </c>
       <c r="C8" s="22" t="n">
-        <f aca="false">[29]output_table!G3/100</f>
-        <v>-0.543372392480144</v>
+        <f aca="false">[17]output_table!G3/100</f>
+        <v>-0.588402847932354</v>
       </c>
       <c r="D8" s="23" t="n">
-        <f aca="false">[29]output_table!H3/100</f>
-        <v>0.298997571056286</v>
+        <f aca="false">[17]output_table!H3/100</f>
+        <v>0.0857004270689324</v>
       </c>
       <c r="E8" s="21" t="n">
-        <f aca="false">[30]output_table!F3/100</f>
-        <v>-0.228230753231275</v>
+        <f aca="false">[18]output_table!F3/100</f>
+        <v>-0.416684080682788</v>
       </c>
       <c r="F8" s="22" t="n">
-        <f aca="false">[30]output_table!G3/100</f>
-        <v>0.156385428602272</v>
+        <f aca="false">[18]output_table!G3/100</f>
+        <v>-0.806512346701537</v>
       </c>
       <c r="G8" s="23" t="n">
-        <f aca="false">[30]output_table!H3/100</f>
-        <v>-0.384616181833547</v>
+        <f aca="false">[18]output_table!H3/100</f>
+        <v>0.389828266018749</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30257,28 +30278,28 @@
         <v>93</v>
       </c>
       <c r="B9" s="21" t="n">
-        <f aca="false">[29]output_table!F4/100</f>
-        <v>-0.519067343614722</v>
+        <f aca="false">[17]output_table!F4/100</f>
+        <v>-0.754604247091419</v>
       </c>
       <c r="C9" s="22" t="n">
-        <f aca="false">[29]output_table!G4/100</f>
-        <v>-1.20014431542971</v>
+        <f aca="false">[17]output_table!G4/100</f>
+        <v>-0.327713766296395</v>
       </c>
       <c r="D9" s="23" t="n">
-        <f aca="false">[29]output_table!H4/100</f>
-        <v>0.681076971814993</v>
+        <f aca="false">[17]output_table!H4/100</f>
+        <v>-0.426890480795024</v>
       </c>
       <c r="E9" s="21" t="n">
-        <f aca="false">[30]output_table!F4/100</f>
-        <v>-0.77417062133289</v>
+        <f aca="false">[18]output_table!F4/100</f>
+        <v>-0.618351738247193</v>
       </c>
       <c r="F9" s="22" t="n">
-        <f aca="false">[30]output_table!G4/100</f>
-        <v>0.376039161400117</v>
+        <f aca="false">[18]output_table!G4/100</f>
+        <v>-0.685256528686372</v>
       </c>
       <c r="G9" s="23" t="n">
-        <f aca="false">[30]output_table!H4/100</f>
-        <v>-1.15020978273301</v>
+        <f aca="false">[18]output_table!H4/100</f>
+        <v>0.0669047904391785</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30286,28 +30307,28 @@
         <v>94</v>
       </c>
       <c r="B10" s="21" t="n">
-        <f aca="false">[29]output_table!F5/100</f>
-        <v>-0.580690718007581</v>
+        <f aca="false">[17]output_table!F5/100</f>
+        <v>-0.769039646345329</v>
       </c>
       <c r="C10" s="22" t="n">
-        <f aca="false">[29]output_table!G5/100</f>
-        <v>-0.799086805784265</v>
+        <f aca="false">[17]output_table!G5/100</f>
+        <v>-0.549844897443001</v>
       </c>
       <c r="D10" s="23" t="n">
-        <f aca="false">[29]output_table!H5/100</f>
-        <v>0.218396087776684</v>
+        <f aca="false">[17]output_table!H5/100</f>
+        <v>-0.219194748902328</v>
       </c>
       <c r="E10" s="21" t="n">
-        <f aca="false">[30]output_table!F5/100</f>
-        <v>-0.813742436866602</v>
+        <f aca="false">[18]output_table!F5/100</f>
+        <v>-0.678704614714606</v>
       </c>
       <c r="F10" s="22" t="n">
-        <f aca="false">[30]output_table!G5/100</f>
-        <v>-1.14810123085594</v>
+        <f aca="false">[18]output_table!G5/100</f>
+        <v>-0.755850938906485</v>
       </c>
       <c r="G10" s="23" t="n">
-        <f aca="false">[30]output_table!H5/100</f>
-        <v>0.334358793989334</v>
+        <f aca="false">[18]output_table!H5/100</f>
+        <v>0.0771463241918783</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30315,28 +30336,28 @@
         <v>95</v>
       </c>
       <c r="B11" s="21" t="n">
-        <f aca="false">[29]output_table!F6/100</f>
-        <v>0.00148798216700991</v>
+        <f aca="false">[17]output_table!F6/100</f>
+        <v>0.0182813106553456</v>
       </c>
       <c r="C11" s="22" t="n">
-        <f aca="false">[29]output_table!G6/100</f>
-        <v>-0.00517503332565823</v>
+        <f aca="false">[17]output_table!G6/100</f>
+        <v>-0.0684938272436293</v>
       </c>
       <c r="D11" s="23" t="n">
-        <f aca="false">[29]output_table!H6/100</f>
-        <v>0.00666301549266814</v>
+        <f aca="false">[17]output_table!H6/100</f>
+        <v>0.0867751378989749</v>
       </c>
       <c r="E11" s="21" t="n">
-        <f aca="false">[30]output_table!F6/100</f>
-        <v>-0.00227964164184585</v>
+        <f aca="false">[18]output_table!F6/100</f>
+        <v>0.00761017944259593</v>
       </c>
       <c r="F11" s="22" t="n">
-        <f aca="false">[30]output_table!G6/100</f>
-        <v>0.0188861176725159</v>
+        <f aca="false">[18]output_table!G6/100</f>
+        <v>0.00151865848969158</v>
       </c>
       <c r="G11" s="23" t="n">
-        <f aca="false">[30]output_table!H6/100</f>
-        <v>-0.0211657593143618</v>
+        <f aca="false">[18]output_table!H6/100</f>
+        <v>0.00609152095290436</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30344,28 +30365,28 @@
         <v>96</v>
       </c>
       <c r="B12" s="21" t="n">
-        <f aca="false">[29]output_table!F7/100</f>
-        <v>-0.142564850715132</v>
+        <f aca="false">[17]output_table!F7/100</f>
+        <v>-0.566601441804896</v>
       </c>
       <c r="C12" s="22" t="n">
-        <f aca="false">[29]output_table!G7/100</f>
-        <v>-0.530229168922839</v>
+        <f aca="false">[17]output_table!G7/100</f>
+        <v>-1.90321986540188</v>
       </c>
       <c r="D12" s="23" t="n">
-        <f aca="false">[29]output_table!H7/100</f>
-        <v>0.387664318207707</v>
+        <f aca="false">[17]output_table!H7/100</f>
+        <v>1.33661842359698</v>
       </c>
       <c r="E12" s="21" t="n">
-        <f aca="false">[30]output_table!F7/100</f>
-        <v>-0.603481275834134</v>
+        <f aca="false">[18]output_table!F7/100</f>
+        <v>-0.322614192993616</v>
       </c>
       <c r="F12" s="22" t="n">
-        <f aca="false">[30]output_table!G7/100</f>
-        <v>-0.424098633842026</v>
+        <f aca="false">[18]output_table!G7/100</f>
+        <v>-0.334786565384342</v>
       </c>
       <c r="G12" s="23" t="n">
-        <f aca="false">[30]output_table!H7/100</f>
-        <v>-0.179382641992108</v>
+        <f aca="false">[18]output_table!H7/100</f>
+        <v>0.0121723723907263</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30373,28 +30394,28 @@
         <v>97</v>
       </c>
       <c r="B13" s="21" t="n">
-        <f aca="false">[29]output_table!F8/100</f>
-        <v>-0.492452883411108</v>
+        <f aca="false">[17]output_table!F8/100</f>
+        <v>-0.800138856686181</v>
       </c>
       <c r="C13" s="22" t="n">
-        <f aca="false">[29]output_table!G8/100</f>
-        <v>-0.37966738886339</v>
+        <f aca="false">[17]output_table!G8/100</f>
+        <v>-0.118707034251192</v>
       </c>
       <c r="D13" s="23" t="n">
-        <f aca="false">[29]output_table!H8/100</f>
-        <v>-0.112785494547718</v>
+        <f aca="false">[17]output_table!H8/100</f>
+        <v>-0.681431822434988</v>
       </c>
       <c r="E13" s="21" t="n">
-        <f aca="false">[30]output_table!F8/100</f>
-        <v>-0.805623863063795</v>
+        <f aca="false">[18]output_table!F8/100</f>
+        <v>-0.739941720766543</v>
       </c>
       <c r="F13" s="22" t="n">
-        <f aca="false">[30]output_table!G8/100</f>
-        <v>0.222387408478649</v>
+        <f aca="false">[18]output_table!G8/100</f>
+        <v>-0.441657827097308</v>
       </c>
       <c r="G13" s="23" t="n">
-        <f aca="false">[30]output_table!H8/100</f>
-        <v>-1.02801127154244</v>
+        <f aca="false">[18]output_table!H8/100</f>
+        <v>-0.298283893669235</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30402,28 +30423,28 @@
         <v>98</v>
       </c>
       <c r="B14" s="21" t="n">
-        <f aca="false">[29]output_table!F9/100</f>
-        <v>-0.277226086616764</v>
+        <f aca="false">[17]output_table!F9/100</f>
+        <v>-0.416616411332547</v>
       </c>
       <c r="C14" s="22" t="n">
-        <f aca="false">[29]output_table!G9/100</f>
-        <v>-0.545526515343252</v>
+        <f aca="false">[17]output_table!G9/100</f>
+        <v>-0.234405608368549</v>
       </c>
       <c r="D14" s="23" t="n">
-        <f aca="false">[29]output_table!H9/100</f>
-        <v>0.268300428726488</v>
+        <f aca="false">[17]output_table!H9/100</f>
+        <v>-0.182210802963999</v>
       </c>
       <c r="E14" s="21" t="n">
-        <f aca="false">[30]output_table!F9/100</f>
-        <v>-0.102549710959205</v>
+        <f aca="false">[18]output_table!F9/100</f>
+        <v>-0.362862348876865</v>
       </c>
       <c r="F14" s="22" t="n">
-        <f aca="false">[30]output_table!G9/100</f>
-        <v>-0.0219850232691694</v>
+        <f aca="false">[18]output_table!G9/100</f>
+        <v>-0.439959968702868</v>
       </c>
       <c r="G14" s="23" t="n">
-        <f aca="false">[30]output_table!H9/100</f>
-        <v>-0.0805646876900356</v>
+        <f aca="false">[18]output_table!H9/100</f>
+        <v>0.0770976198260029</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30431,28 +30452,28 @@
         <v>99</v>
       </c>
       <c r="B15" s="21" t="n">
-        <f aca="false">[29]output_table!F10/100</f>
-        <v>-0.113835253898429</v>
+        <f aca="false">[17]output_table!F10/100</f>
+        <v>-0.276058793004082</v>
       </c>
       <c r="C15" s="22" t="n">
-        <f aca="false">[29]output_table!G10/100</f>
-        <v>0.0410072534058516</v>
+        <f aca="false">[17]output_table!G10/100</f>
+        <v>0.561379934275976</v>
       </c>
       <c r="D15" s="23" t="n">
-        <f aca="false">[29]output_table!H10/100</f>
-        <v>-0.15484250730428</v>
+        <f aca="false">[17]output_table!H10/100</f>
+        <v>-0.837438727280057</v>
       </c>
       <c r="E15" s="21" t="n">
-        <f aca="false">[30]output_table!F10/100</f>
-        <v>0.199010897848067</v>
+        <f aca="false">[18]output_table!F10/100</f>
+        <v>-0.195022920583921</v>
       </c>
       <c r="F15" s="22" t="n">
-        <f aca="false">[30]output_table!G10/100</f>
-        <v>0.837714983171599</v>
+        <f aca="false">[18]output_table!G10/100</f>
+        <v>0.229354732647409</v>
       </c>
       <c r="G15" s="23" t="n">
-        <f aca="false">[30]output_table!H10/100</f>
-        <v>-0.638704085323531</v>
+        <f aca="false">[18]output_table!H10/100</f>
+        <v>-0.42437765323133</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30460,28 +30481,28 @@
         <v>100</v>
       </c>
       <c r="B16" s="21" t="n">
-        <f aca="false">[29]output_table!F11/100</f>
-        <v>-0.193471852953465</v>
+        <f aca="false">[17]output_table!F11/100</f>
+        <v>-0.527757329740792</v>
       </c>
       <c r="C16" s="22" t="n">
-        <f aca="false">[29]output_table!G11/100</f>
-        <v>-0.255467838279911</v>
+        <f aca="false">[17]output_table!G11/100</f>
+        <v>-0.0518258098908403</v>
       </c>
       <c r="D16" s="23" t="n">
-        <f aca="false">[29]output_table!H11/100</f>
-        <v>0.0619959853264459</v>
+        <f aca="false">[17]output_table!H11/100</f>
+        <v>-0.475931519849952</v>
       </c>
       <c r="E16" s="21" t="n">
-        <f aca="false">[30]output_table!F11/100</f>
-        <v>1.57632433295042</v>
+        <f aca="false">[18]output_table!F11/100</f>
+        <v>-0.502685713897412</v>
       </c>
       <c r="F16" s="22" t="n">
-        <f aca="false">[30]output_table!G11/100</f>
-        <v>0.479272941067823</v>
+        <f aca="false">[18]output_table!G11/100</f>
+        <v>-0.595439688399256</v>
       </c>
       <c r="G16" s="23" t="n">
-        <f aca="false">[30]output_table!H11/100</f>
-        <v>1.0970513918826</v>
+        <f aca="false">[18]output_table!H11/100</f>
+        <v>0.092753974501844</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30489,28 +30510,28 @@
         <v>101</v>
       </c>
       <c r="B17" s="21" t="n">
-        <f aca="false">[29]output_table!F12/100</f>
-        <v>-0.196861749866989</v>
+        <f aca="false">[17]output_table!F12/100</f>
+        <v>-0.421403214905773</v>
       </c>
       <c r="C17" s="22" t="n">
-        <f aca="false">[29]output_table!G12/100</f>
-        <v>-0.0233002931491005</v>
+        <f aca="false">[17]output_table!G12/100</f>
+        <v>0.699629814316786</v>
       </c>
       <c r="D17" s="23" t="n">
-        <f aca="false">[29]output_table!H12/100</f>
-        <v>-0.173561456717888</v>
+        <f aca="false">[17]output_table!H12/100</f>
+        <v>-1.12103302922256</v>
       </c>
       <c r="E17" s="21" t="n">
-        <f aca="false">[30]output_table!F12/100</f>
-        <v>-0.158048493772097</v>
+        <f aca="false">[18]output_table!F12/100</f>
+        <v>-0.0418007322504184</v>
       </c>
       <c r="F17" s="22" t="n">
-        <f aca="false">[30]output_table!G12/100</f>
-        <v>0.196454646122422</v>
+        <f aca="false">[18]output_table!G12/100</f>
+        <v>0.176776699242765</v>
       </c>
       <c r="G17" s="23" t="n">
-        <f aca="false">[30]output_table!H12/100</f>
-        <v>-0.354503139894518</v>
+        <f aca="false">[18]output_table!H12/100</f>
+        <v>-0.218577431493184</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30518,28 +30539,28 @@
         <v>102</v>
       </c>
       <c r="B18" s="21" t="n">
-        <f aca="false">[29]output_table!F13/100</f>
-        <v>-0.174660605201418</v>
+        <f aca="false">[17]output_table!F13/100</f>
+        <v>-0.390602773113667</v>
       </c>
       <c r="C18" s="22" t="n">
-        <f aca="false">[29]output_table!G13/100</f>
-        <v>-0.0636371613876475</v>
+        <f aca="false">[17]output_table!G13/100</f>
+        <v>-0.184949753724605</v>
       </c>
       <c r="D18" s="23" t="n">
-        <f aca="false">[29]output_table!H13/100</f>
-        <v>-0.11102344381377</v>
+        <f aca="false">[17]output_table!H13/100</f>
+        <v>-0.205653019389062</v>
       </c>
       <c r="E18" s="21" t="n">
-        <f aca="false">[30]output_table!F13/100</f>
-        <v>-0.0749476493598397</v>
+        <f aca="false">[18]output_table!F13/100</f>
+        <v>-0.0622459164831054</v>
       </c>
       <c r="F18" s="22" t="n">
-        <f aca="false">[30]output_table!G13/100</f>
-        <v>-0.00779280541311926</v>
+        <f aca="false">[18]output_table!G13/100</f>
+        <v>-0.0202188255754279</v>
       </c>
       <c r="G18" s="23" t="n">
-        <f aca="false">[30]output_table!H13/100</f>
-        <v>-0.0671548439467204</v>
+        <f aca="false">[18]output_table!H13/100</f>
+        <v>-0.0420270909076775</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30547,28 +30568,28 @@
         <v>103</v>
       </c>
       <c r="B19" s="21" t="n">
-        <f aca="false">[29]output_table!F14/100</f>
-        <v>-0.423678389613345</v>
+        <f aca="false">[17]output_table!F14/100</f>
+        <v>-0.603826540757764</v>
       </c>
       <c r="C19" s="22" t="n">
-        <f aca="false">[29]output_table!G14/100</f>
-        <v>-0.509302170187423</v>
+        <f aca="false">[17]output_table!G14/100</f>
+        <v>-0.226213245775179</v>
       </c>
       <c r="D19" s="23" t="n">
-        <f aca="false">[29]output_table!H14/100</f>
-        <v>0.0856237805740784</v>
+        <f aca="false">[17]output_table!H14/100</f>
+        <v>-0.377613294982585</v>
       </c>
       <c r="E19" s="21" t="n">
-        <f aca="false">[30]output_table!F14/100</f>
-        <v>-0.315300992401331</v>
+        <f aca="false">[18]output_table!F14/100</f>
+        <v>-0.593220758737135</v>
       </c>
       <c r="F19" s="22" t="n">
-        <f aca="false">[30]output_table!G14/100</f>
-        <v>-0.237501064971338</v>
+        <f aca="false">[18]output_table!G14/100</f>
+        <v>-0.518659697057861</v>
       </c>
       <c r="G19" s="23" t="n">
-        <f aca="false">[30]output_table!H14/100</f>
-        <v>-0.0777999274299929</v>
+        <f aca="false">[18]output_table!H14/100</f>
+        <v>-0.074561061679274</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30576,28 +30597,28 @@
         <v>104</v>
       </c>
       <c r="B20" s="21" t="n">
-        <f aca="false">[29]output_table!F15/100</f>
-        <v>-0.106176015864681</v>
+        <f aca="false">[17]output_table!F15/100</f>
+        <v>-0.311829960577724</v>
       </c>
       <c r="C20" s="22" t="n">
-        <f aca="false">[29]output_table!G15/100</f>
-        <v>0.0304484286407378</v>
+        <f aca="false">[17]output_table!G15/100</f>
+        <v>0.553170195400885</v>
       </c>
       <c r="D20" s="23" t="n">
-        <f aca="false">[29]output_table!H15/100</f>
-        <v>-0.136624444505419</v>
+        <f aca="false">[17]output_table!H15/100</f>
+        <v>-0.865000155978609</v>
       </c>
       <c r="E20" s="21" t="n">
-        <f aca="false">[30]output_table!F15/100</f>
-        <v>-0.0549753947063335</v>
+        <f aca="false">[18]output_table!F15/100</f>
+        <v>-0.211747256800595</v>
       </c>
       <c r="F20" s="22" t="n">
-        <f aca="false">[30]output_table!G15/100</f>
-        <v>0.65937894183685</v>
+        <f aca="false">[18]output_table!G15/100</f>
+        <v>0.206559022504728</v>
       </c>
       <c r="G20" s="23" t="n">
-        <f aca="false">[30]output_table!H15/100</f>
-        <v>-0.714354336543184</v>
+        <f aca="false">[18]output_table!H15/100</f>
+        <v>-0.418306279305323</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30605,28 +30626,28 @@
         <v>105</v>
       </c>
       <c r="B21" s="21" t="n">
-        <f aca="false">[29]output_table!F16/100</f>
-        <v>0.0296940293156509</v>
+        <f aca="false">[17]output_table!F16/100</f>
+        <v>-0.0239769981678716</v>
       </c>
       <c r="C21" s="22" t="n">
-        <f aca="false">[29]output_table!G16/100</f>
-        <v>0.00754191321264443</v>
+        <f aca="false">[17]output_table!G16/100</f>
+        <v>0.164710157286001</v>
       </c>
       <c r="D21" s="23" t="n">
-        <f aca="false">[29]output_table!H16/100</f>
-        <v>0.0221521161030064</v>
+        <f aca="false">[17]output_table!H16/100</f>
+        <v>-0.188687155453873</v>
       </c>
       <c r="E21" s="21" t="n">
-        <f aca="false">[30]output_table!F16/100</f>
-        <v>0.079719948086892</v>
+        <f aca="false">[18]output_table!F16/100</f>
+        <v>-0.0108342431981264</v>
       </c>
       <c r="F21" s="22" t="n">
-        <f aca="false">[30]output_table!G16/100</f>
-        <v>0.173708435483298</v>
+        <f aca="false">[18]output_table!G16/100</f>
+        <v>0.0468465218392612</v>
       </c>
       <c r="G21" s="23" t="n">
-        <f aca="false">[30]output_table!H16/100</f>
-        <v>-0.0939884873964065</v>
+        <f aca="false">[18]output_table!H16/100</f>
+        <v>-0.0576807650373878</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30634,28 +30655,28 @@
         <v>106</v>
       </c>
       <c r="B22" s="21" t="n">
-        <f aca="false">[29]output_table!F17/100</f>
-        <v>-0.467974722117531</v>
+        <f aca="false">[17]output_table!F17/100</f>
+        <v>-0.714490451736532</v>
       </c>
       <c r="C22" s="22" t="n">
-        <f aca="false">[29]output_table!G17/100</f>
-        <v>-0.578010968696742</v>
+        <f aca="false">[17]output_table!G17/100</f>
+        <v>-0.275872663100018</v>
       </c>
       <c r="D22" s="23" t="n">
-        <f aca="false">[29]output_table!H17/100</f>
-        <v>0.110036246579211</v>
+        <f aca="false">[17]output_table!H17/100</f>
+        <v>-0.438617788636514</v>
       </c>
       <c r="E22" s="21" t="n">
-        <f aca="false">[30]output_table!F17/100</f>
-        <v>-0.331043806473291</v>
+        <f aca="false">[18]output_table!F17/100</f>
+        <v>-0.455866497568974</v>
       </c>
       <c r="F22" s="22" t="n">
-        <f aca="false">[30]output_table!G17/100</f>
-        <v>-0.655061779791485</v>
+        <f aca="false">[18]output_table!G17/100</f>
+        <v>-0.488027441113953</v>
       </c>
       <c r="G22" s="23" t="n">
-        <f aca="false">[30]output_table!H17/100</f>
-        <v>0.324017973318194</v>
+        <f aca="false">[18]output_table!H17/100</f>
+        <v>0.0321609435449784</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30663,28 +30684,28 @@
         <v>107</v>
       </c>
       <c r="B23" s="21" t="n">
-        <f aca="false">[29]output_table!F18/100</f>
-        <v>-0.398552026477866</v>
+        <f aca="false">[17]output_table!F18/100</f>
+        <v>-0.777242558035879</v>
       </c>
       <c r="C23" s="22" t="n">
-        <f aca="false">[29]output_table!G18/100</f>
-        <v>-0.912143662445799</v>
+        <f aca="false">[17]output_table!G18/100</f>
+        <v>-0.379692833960334</v>
       </c>
       <c r="D23" s="23" t="n">
-        <f aca="false">[29]output_table!H18/100</f>
-        <v>0.513591635967933</v>
+        <f aca="false">[17]output_table!H18/100</f>
+        <v>-0.397549724075545</v>
       </c>
       <c r="E23" s="21" t="n">
-        <f aca="false">[30]output_table!F18/100</f>
-        <v>-0.347105652883372</v>
+        <f aca="false">[18]output_table!F18/100</f>
+        <v>-0.689380336386343</v>
       </c>
       <c r="F23" s="22" t="n">
-        <f aca="false">[30]output_table!G18/100</f>
-        <v>-0.188868133215729</v>
+        <f aca="false">[18]output_table!G18/100</f>
+        <v>-0.889750248849365</v>
       </c>
       <c r="G23" s="23" t="n">
-        <f aca="false">[30]output_table!H18/100</f>
-        <v>-0.158237519667643</v>
+        <f aca="false">[18]output_table!H18/100</f>
+        <v>0.200369912463023</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30692,28 +30713,28 @@
         <v>108</v>
       </c>
       <c r="B24" s="21" t="n">
-        <f aca="false">[29]output_table!F19/100</f>
-        <v>-0.205316753152855</v>
+        <f aca="false">[17]output_table!F19/100</f>
+        <v>-0.328139110095778</v>
       </c>
       <c r="C24" s="22" t="n">
-        <f aca="false">[29]output_table!G19/100</f>
-        <v>-0.889409467706447</v>
+        <f aca="false">[17]output_table!G19/100</f>
+        <v>-0.54693192934407</v>
       </c>
       <c r="D24" s="23" t="n">
-        <f aca="false">[29]output_table!H19/100</f>
-        <v>0.684092714553592</v>
+        <f aca="false">[17]output_table!H19/100</f>
+        <v>0.218792819248292</v>
       </c>
       <c r="E24" s="21" t="n">
-        <f aca="false">[30]output_table!F19/100</f>
-        <v>-0.382826257083383</v>
+        <f aca="false">[18]output_table!F19/100</f>
+        <v>-0.360600107403677</v>
       </c>
       <c r="F24" s="22" t="n">
-        <f aca="false">[30]output_table!G19/100</f>
-        <v>-0.377981614204648</v>
+        <f aca="false">[18]output_table!G19/100</f>
+        <v>-0.629796204238378</v>
       </c>
       <c r="G24" s="23" t="n">
-        <f aca="false">[30]output_table!H19/100</f>
-        <v>-0.00484464287873454</v>
+        <f aca="false">[18]output_table!H19/100</f>
+        <v>0.269196096834701</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30721,28 +30742,28 @@
         <v>109</v>
       </c>
       <c r="B25" s="21" t="n">
-        <f aca="false">[29]output_table!F20/100</f>
-        <v>-0.0448722535326793</v>
+        <f aca="false">[17]output_table!F20/100</f>
+        <v>-0.201935445388272</v>
       </c>
       <c r="C25" s="22" t="n">
-        <f aca="false">[29]output_table!G20/100</f>
-        <v>-0.496369095325512</v>
+        <f aca="false">[17]output_table!G20/100</f>
+        <v>-0.070205522438127</v>
       </c>
       <c r="D25" s="23" t="n">
-        <f aca="false">[29]output_table!H20/100</f>
-        <v>0.451496841792833</v>
+        <f aca="false">[17]output_table!H20/100</f>
+        <v>-0.131729922950144</v>
       </c>
       <c r="E25" s="21" t="n">
-        <f aca="false">[30]output_table!F20/100</f>
-        <v>-0.0582872078297532</v>
+        <f aca="false">[18]output_table!F20/100</f>
+        <v>-0.0034493809491938</v>
       </c>
       <c r="F25" s="22" t="n">
-        <f aca="false">[30]output_table!G20/100</f>
-        <v>1.6623371979197</v>
+        <f aca="false">[18]output_table!G20/100</f>
+        <v>-0.423712662360076</v>
       </c>
       <c r="G25" s="23" t="n">
-        <f aca="false">[30]output_table!H20/100</f>
-        <v>-1.72062440574945</v>
+        <f aca="false">[18]output_table!H20/100</f>
+        <v>0.420263281410882</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30750,28 +30771,28 @@
         <v>110</v>
       </c>
       <c r="B26" s="21" t="n">
-        <f aca="false">[29]output_table!F21/100</f>
-        <v>0.0242106592073112</v>
+        <f aca="false">[17]output_table!F21/100</f>
+        <v>0.0405489812284114</v>
       </c>
       <c r="C26" s="22" t="n">
-        <f aca="false">[29]output_table!G21/100</f>
-        <v>-0.0458193011121156</v>
+        <f aca="false">[17]output_table!G21/100</f>
+        <v>-0.057669814061569</v>
       </c>
       <c r="D26" s="23" t="n">
-        <f aca="false">[29]output_table!H21/100</f>
-        <v>0.0700299603194268</v>
+        <f aca="false">[17]output_table!H21/100</f>
+        <v>0.0982187952899806</v>
       </c>
       <c r="E26" s="21" t="n">
-        <f aca="false">[30]output_table!F21/100</f>
-        <v>0.0264858142588495</v>
+        <f aca="false">[18]output_table!F21/100</f>
+        <v>-0.00272427443717159</v>
       </c>
       <c r="F26" s="22" t="n">
-        <f aca="false">[30]output_table!G21/100</f>
-        <v>0.106312081109899</v>
+        <f aca="false">[18]output_table!G21/100</f>
+        <v>-0.0347716281465467</v>
       </c>
       <c r="G26" s="23" t="n">
-        <f aca="false">[30]output_table!H21/100</f>
-        <v>-0.0798262668510493</v>
+        <f aca="false">[18]output_table!H21/100</f>
+        <v>0.0320473537093751</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30779,28 +30800,28 @@
         <v>111</v>
       </c>
       <c r="B27" s="21" t="n">
-        <f aca="false">[29]output_table!F22/100</f>
-        <v>-0.0145737451200485</v>
-      </c>
-      <c r="C27" s="22" t="n">
-        <f aca="false">[29]output_table!G22/100</f>
-        <v>-0.0798375863200927</v>
-      </c>
-      <c r="D27" s="23" t="n">
-        <f aca="false">[29]output_table!H22/100</f>
-        <v>0.0652638412000442</v>
+        <f aca="false">[17]output_table!F22/100</f>
+        <v>0.0124804916893947</v>
+      </c>
+      <c r="C27" s="36" t="n">
+        <f aca="false">[17]output_table!G22/100</f>
+        <v>-13.9365629943119</v>
+      </c>
+      <c r="D27" s="37" t="n">
+        <f aca="false">[17]output_table!H22/100</f>
+        <v>13.9490434860013</v>
       </c>
       <c r="E27" s="21" t="n">
-        <f aca="false">[30]output_table!F22/100</f>
-        <v>0.792225852507143</v>
+        <f aca="false">[18]output_table!F22/100</f>
+        <v>0.00624883185251995</v>
       </c>
       <c r="F27" s="22" t="n">
-        <f aca="false">[30]output_table!G22/100</f>
-        <v>0.807671138129608</v>
+        <f aca="false">[18]output_table!G22/100</f>
+        <v>-0.0156291315252097</v>
       </c>
       <c r="G27" s="23" t="n">
-        <f aca="false">[30]output_table!H22/100</f>
-        <v>-0.0154452856224645</v>
+        <f aca="false">[18]output_table!H22/100</f>
+        <v>0.0218779633777296</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30808,28 +30829,28 @@
         <v>112</v>
       </c>
       <c r="B28" s="21" t="n">
-        <f aca="false">[29]output_table!F23/100</f>
-        <v>-0.380717854226395</v>
+        <f aca="false">[17]output_table!F23/100</f>
+        <v>-0.844632238182775</v>
       </c>
       <c r="C28" s="22" t="n">
-        <f aca="false">[29]output_table!G23/100</f>
-        <v>-0.245862184231078</v>
+        <f aca="false">[17]output_table!G23/100</f>
+        <v>-0.276165975484058</v>
       </c>
       <c r="D28" s="23" t="n">
-        <f aca="false">[29]output_table!H23/100</f>
-        <v>-0.134855669995317</v>
+        <f aca="false">[17]output_table!H23/100</f>
+        <v>-0.568466262698718</v>
       </c>
       <c r="E28" s="21" t="n">
-        <f aca="false">[30]output_table!F23/100</f>
-        <v>-0.533366574083791</v>
+        <f aca="false">[18]output_table!F23/100</f>
+        <v>-0.733969487507731</v>
       </c>
       <c r="F28" s="22" t="n">
-        <f aca="false">[30]output_table!G23/100</f>
-        <v>0.339166529569355</v>
+        <f aca="false">[18]output_table!G23/100</f>
+        <v>-0.479863715239884</v>
       </c>
       <c r="G28" s="23" t="n">
-        <f aca="false">[30]output_table!H23/100</f>
-        <v>-0.872533103653146</v>
+        <f aca="false">[18]output_table!H23/100</f>
+        <v>-0.254105772267847</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30837,28 +30858,28 @@
         <v>113</v>
       </c>
       <c r="B29" s="21" t="n">
-        <f aca="false">[29]output_table!F24/100</f>
-        <v>-0.307753648851186</v>
+        <f aca="false">[17]output_table!F24/100</f>
+        <v>-0.482109191480942</v>
       </c>
       <c r="C29" s="22" t="n">
-        <f aca="false">[29]output_table!G24/100</f>
-        <v>-0.356293815819547</v>
+        <f aca="false">[17]output_table!G24/100</f>
+        <v>0.263421457661312</v>
       </c>
       <c r="D29" s="23" t="n">
-        <f aca="false">[29]output_table!H24/100</f>
-        <v>0.0485401669683606</v>
+        <f aca="false">[17]output_table!H24/100</f>
+        <v>-0.745530649142253</v>
       </c>
       <c r="E29" s="21" t="n">
-        <f aca="false">[30]output_table!F24/100</f>
-        <v>0.340016562998975</v>
+        <f aca="false">[18]output_table!F24/100</f>
+        <v>-0.381263086841299</v>
       </c>
       <c r="F29" s="22" t="n">
-        <f aca="false">[30]output_table!G24/100</f>
-        <v>0.465582311452327</v>
+        <f aca="false">[18]output_table!G24/100</f>
+        <v>-0.00413882276424571</v>
       </c>
       <c r="G29" s="23" t="n">
-        <f aca="false">[30]output_table!H24/100</f>
-        <v>-0.125565748453352</v>
+        <f aca="false">[18]output_table!H24/100</f>
+        <v>-0.377124264077053</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30866,28 +30887,28 @@
         <v>114</v>
       </c>
       <c r="B30" s="21" t="n">
-        <f aca="false">[29]output_table!F25/100</f>
-        <v>-0.282944435893703</v>
+        <f aca="false">[17]output_table!F25/100</f>
+        <v>-0.659916346739682</v>
       </c>
       <c r="C30" s="22" t="n">
-        <f aca="false">[29]output_table!G25/100</f>
-        <v>-0.209917282784647</v>
+        <f aca="false">[17]output_table!G25/100</f>
+        <v>0.0914574639988598</v>
       </c>
       <c r="D30" s="23" t="n">
-        <f aca="false">[29]output_table!H25/100</f>
-        <v>-0.0730271531090558</v>
+        <f aca="false">[17]output_table!H25/100</f>
+        <v>-0.751373810738542</v>
       </c>
       <c r="E30" s="21" t="n">
-        <f aca="false">[30]output_table!F25/100</f>
-        <v>-0.00387560202024685</v>
+        <f aca="false">[18]output_table!F25/100</f>
+        <v>-0.536629909352087</v>
       </c>
       <c r="F30" s="22" t="n">
-        <f aca="false">[30]output_table!G25/100</f>
-        <v>1.14323422022419</v>
+        <f aca="false">[18]output_table!G25/100</f>
+        <v>-0.279887122120898</v>
       </c>
       <c r="G30" s="23" t="n">
-        <f aca="false">[30]output_table!H25/100</f>
-        <v>-1.14710982224443</v>
+        <f aca="false">[18]output_table!H25/100</f>
+        <v>-0.25674278723119</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30895,28 +30916,28 @@
         <v>115</v>
       </c>
       <c r="B31" s="25" t="n">
-        <f aca="false">[29]output_table!F26/100</f>
-        <v>0.00274887888504036</v>
+        <f aca="false">[17]output_table!F26/100</f>
+        <v>-0.013417262111894</v>
       </c>
       <c r="C31" s="26" t="n">
-        <f aca="false">[29]output_table!G26/100</f>
-        <v>0.00483104676231486</v>
+        <f aca="false">[17]output_table!G26/100</f>
+        <v>0.149561161589925</v>
       </c>
       <c r="D31" s="27" t="n">
-        <f aca="false">[29]output_table!H26/100</f>
-        <v>-0.0020821678772745</v>
+        <f aca="false">[17]output_table!H26/100</f>
+        <v>-0.162978423701819</v>
       </c>
       <c r="E31" s="25" t="n">
-        <f aca="false">[30]output_table!F26/100</f>
-        <v>0.210206312128304</v>
+        <f aca="false">[18]output_table!F26/100</f>
+        <v>-0.00550271986507331</v>
       </c>
       <c r="F31" s="26" t="n">
-        <f aca="false">[30]output_table!G26/100</f>
-        <v>0.359960903355552</v>
+        <f aca="false">[18]output_table!G26/100</f>
+        <v>0.00487407204935892</v>
       </c>
       <c r="G31" s="27" t="n">
-        <f aca="false">[30]output_table!H26/100</f>
-        <v>-0.149754591227248</v>
+        <f aca="false">[18]output_table!H26/100</f>
+        <v>-0.0103767919144322</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30925,27 +30946,27 @@
       </c>
       <c r="B32" s="28" t="n">
         <f aca="false">AVERAGE(B7:B31)</f>
-        <v>-0.220733776446165</v>
+        <v>-0.416860210183796</v>
       </c>
       <c r="C32" s="28" t="n">
         <f aca="false">AVERAGE(C7:C31)</f>
-        <v>-0.345303863270306</v>
+        <v>-0.687775647731814</v>
       </c>
       <c r="D32" s="28" t="n">
         <f aca="false">AVERAGE(D7:D31)</f>
-        <v>0.124570086824141</v>
+        <v>0.270915437548018</v>
       </c>
       <c r="E32" s="28" t="n">
         <f aca="false">AVERAGE(E7:E31)</f>
-        <v>-0.0975286194354516</v>
+        <v>-0.316811225238152</v>
       </c>
       <c r="F32" s="28" t="n">
         <f aca="false">AVERAGE(F7:F31)</f>
-        <v>0.20722988792682</v>
+        <v>-0.287716148054257</v>
       </c>
       <c r="G32" s="28" t="n">
         <f aca="false">AVERAGE(G7:G31)</f>
-        <v>-0.304758507362271</v>
+        <v>-0.0290950771838952</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -31024,19 +31045,19 @@
       <c r="A6" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="36" t="n">
+      <c r="B6" s="38" t="n">
         <f aca="false">ROUND([53]output_table!b2,6)</f>
         <v>0.000902</v>
       </c>
-      <c r="C6" s="37" t="n">
+      <c r="C6" s="39" t="n">
         <f aca="false">ROUND([53]output_table!d2,6)</f>
         <v>0.001047</v>
       </c>
-      <c r="D6" s="37" t="n">
+      <c r="D6" s="39" t="n">
         <f aca="false">ROUND([53]output_table!c2,6)</f>
         <v>0.000923</v>
       </c>
-      <c r="E6" s="38" t="n">
+      <c r="E6" s="40" t="n">
         <f aca="false">ROUND([53]output_table!e2,6)</f>
         <v>0.001056</v>
       </c>
@@ -31045,19 +31066,19 @@
       <c r="A7" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="39" t="n">
+      <c r="B7" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b3,6)</f>
         <v>0.000537</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d3,6)</f>
         <v>0.00069</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c3,6)</f>
         <v>0.000948</v>
       </c>
-      <c r="E7" s="41" t="n">
+      <c r="E7" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e3,6)</f>
         <v>0.001807</v>
       </c>
@@ -31066,19 +31087,19 @@
       <c r="A8" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="39" t="n">
+      <c r="B8" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b4,6)</f>
         <v>0.001022</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d4,6)</f>
         <v>0.001122</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c4,6)</f>
         <v>0.00301</v>
       </c>
-      <c r="E8" s="41" t="n">
+      <c r="E8" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e4,6)</f>
         <v>0.00435</v>
       </c>
@@ -31087,19 +31108,19 @@
       <c r="A9" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="39" t="n">
+      <c r="B9" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b5,6)</f>
         <v>0.000592</v>
       </c>
-      <c r="C9" s="40" t="n">
+      <c r="C9" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d5,6)</f>
         <v>0.001075</v>
       </c>
-      <c r="D9" s="40" t="n">
+      <c r="D9" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c5,6)</f>
         <v>0.002177</v>
       </c>
-      <c r="E9" s="41" t="n">
+      <c r="E9" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e5,6)</f>
         <v>0.003263</v>
       </c>
@@ -31108,19 +31129,19 @@
       <c r="A10" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="39" t="n">
+      <c r="B10" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b6,6)</f>
         <v>0.006239</v>
       </c>
-      <c r="C10" s="40" t="n">
+      <c r="C10" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d6,6)</f>
         <v>0.007006</v>
       </c>
-      <c r="D10" s="40" t="n">
+      <c r="D10" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c6,6)</f>
         <v>0.006153</v>
       </c>
-      <c r="E10" s="41" t="n">
+      <c r="E10" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e6,6)</f>
         <v>0.006978</v>
       </c>
@@ -31129,19 +31150,19 @@
       <c r="A11" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="39" t="n">
+      <c r="B11" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b7,6)</f>
         <v>0.0011</v>
       </c>
-      <c r="C11" s="40" t="n">
+      <c r="C11" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d7,6)</f>
         <v>0.002508</v>
       </c>
-      <c r="D11" s="40" t="n">
+      <c r="D11" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c7,6)</f>
         <v>0.001943</v>
       </c>
-      <c r="E11" s="41" t="n">
+      <c r="E11" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e7,6)</f>
         <v>0.003776</v>
       </c>
@@ -31150,19 +31171,19 @@
       <c r="A12" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="39" t="n">
+      <c r="B12" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b8,6)</f>
         <v>0.000442</v>
       </c>
-      <c r="C12" s="40" t="n">
+      <c r="C12" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d8,6)</f>
         <v>0.000479</v>
       </c>
-      <c r="D12" s="40" t="n">
+      <c r="D12" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c8,6)</f>
         <v>0.00201</v>
       </c>
-      <c r="E12" s="41" t="n">
+      <c r="E12" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e8,6)</f>
         <v>0.001285</v>
       </c>
@@ -31171,19 +31192,19 @@
       <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="39" t="n">
+      <c r="B13" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b9,6)</f>
         <v>0.000618</v>
       </c>
-      <c r="C13" s="40" t="n">
+      <c r="C13" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d9,6)</f>
         <v>0.001</v>
       </c>
-      <c r="D13" s="40" t="n">
+      <c r="D13" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c9,6)</f>
         <v>0.000992</v>
       </c>
-      <c r="E13" s="41" t="n">
+      <c r="E13" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e9,6)</f>
         <v>0.001661</v>
       </c>
@@ -31192,19 +31213,19 @@
       <c r="A14" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="39" t="n">
+      <c r="B14" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b10,6)</f>
         <v>0.000196</v>
       </c>
-      <c r="C14" s="40" t="n">
+      <c r="C14" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d10,6)</f>
         <v>0.000257</v>
       </c>
-      <c r="D14" s="40" t="n">
+      <c r="D14" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c10,6)</f>
         <v>0.000262</v>
       </c>
-      <c r="E14" s="41" t="n">
+      <c r="E14" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e10,6)</f>
         <v>0.000189</v>
       </c>
@@ -31213,19 +31234,19 @@
       <c r="A15" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="39" t="n">
+      <c r="B15" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b11,6)</f>
         <v>0.000244</v>
       </c>
-      <c r="C15" s="40" t="n">
+      <c r="C15" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d11,6)</f>
         <v>0.000428</v>
       </c>
-      <c r="D15" s="40" t="n">
+      <c r="D15" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c11,6)</f>
         <v>0.00052</v>
       </c>
-      <c r="E15" s="41" t="n">
+      <c r="E15" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e11,6)</f>
         <v>0.000687</v>
       </c>
@@ -31234,19 +31255,19 @@
       <c r="A16" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B16" s="39" t="n">
+      <c r="B16" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b12,6)</f>
         <v>0.000298</v>
       </c>
-      <c r="C16" s="40" t="n">
+      <c r="C16" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d12,6)</f>
         <v>0.00044</v>
       </c>
-      <c r="D16" s="40" t="n">
+      <c r="D16" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c12,6)</f>
         <v>0.000379</v>
       </c>
-      <c r="E16" s="41" t="n">
+      <c r="E16" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e12,6)</f>
         <v>0.000409</v>
       </c>
@@ -31255,19 +31276,19 @@
       <c r="A17" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="39" t="n">
+      <c r="B17" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b13,6)</f>
         <v>0.001019</v>
       </c>
-      <c r="C17" s="40" t="n">
+      <c r="C17" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d13,6)</f>
         <v>0.000861</v>
       </c>
-      <c r="D17" s="40" t="n">
+      <c r="D17" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c13,6)</f>
         <v>0.001213</v>
       </c>
-      <c r="E17" s="41" t="n">
+      <c r="E17" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e13,6)</f>
         <v>0.000936</v>
       </c>
@@ -31276,19 +31297,19 @@
       <c r="A18" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="39" t="n">
+      <c r="B18" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b14,6)</f>
         <v>0.001048</v>
       </c>
-      <c r="C18" s="40" t="n">
+      <c r="C18" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d14,6)</f>
         <v>0.002048</v>
       </c>
-      <c r="D18" s="40" t="n">
+      <c r="D18" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c14,6)</f>
         <v>0.002557</v>
       </c>
-      <c r="E18" s="41" t="n">
+      <c r="E18" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e14,6)</f>
         <v>0.003812</v>
       </c>
@@ -31297,19 +31318,19 @@
       <c r="A19" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="39" t="n">
+      <c r="B19" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b15,6)</f>
         <v>0.00019</v>
       </c>
-      <c r="C19" s="42" t="n">
+      <c r="C19" s="44" t="n">
         <f aca="false">ROUND([53]output_table!d15,6)</f>
         <v>0.000182</v>
       </c>
-      <c r="D19" s="40" t="n">
+      <c r="D19" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c15,6)</f>
         <v>0.000262</v>
       </c>
-      <c r="E19" s="41" t="n">
+      <c r="E19" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e15,6)</f>
         <v>0.000126</v>
       </c>
@@ -31318,19 +31339,19 @@
       <c r="A20" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="39" t="n">
+      <c r="B20" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b16,6)</f>
         <v>0.000296</v>
       </c>
-      <c r="C20" s="40" t="n">
+      <c r="C20" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d16,6)</f>
         <v>0.000223</v>
       </c>
-      <c r="D20" s="40" t="n">
+      <c r="D20" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c16,6)</f>
         <v>0.000305</v>
       </c>
-      <c r="E20" s="41" t="n">
+      <c r="E20" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e16,6)</f>
         <v>0.000199</v>
       </c>
@@ -31339,19 +31360,19 @@
       <c r="A21" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="39" t="n">
+      <c r="B21" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b17,6)</f>
         <v>0.001049</v>
       </c>
-      <c r="C21" s="40" t="n">
+      <c r="C21" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d17,6)</f>
         <v>0.005222</v>
       </c>
-      <c r="D21" s="40" t="n">
+      <c r="D21" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c17,6)</f>
         <v>0.002422</v>
       </c>
-      <c r="E21" s="41" t="n">
+      <c r="E21" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e17,6)</f>
         <v>0.007472</v>
       </c>
@@ -31360,19 +31381,19 @@
       <c r="A22" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="39" t="n">
+      <c r="B22" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b18,6)</f>
         <v>0.000336</v>
       </c>
-      <c r="C22" s="40" t="n">
+      <c r="C22" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d18,6)</f>
         <v>0.000658</v>
       </c>
-      <c r="D22" s="40" t="n">
+      <c r="D22" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c18,6)</f>
         <v>0.001236</v>
       </c>
-      <c r="E22" s="41" t="n">
+      <c r="E22" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e18,6)</f>
         <v>0.002313</v>
       </c>
@@ -31381,19 +31402,19 @@
       <c r="A23" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="39" t="n">
+      <c r="B23" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b19,6)</f>
         <v>0.000842</v>
       </c>
-      <c r="C23" s="40" t="n">
+      <c r="C23" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d19,6)</f>
         <v>0.002089</v>
       </c>
-      <c r="D23" s="40" t="n">
+      <c r="D23" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c19,6)</f>
         <v>0.001259</v>
       </c>
-      <c r="E23" s="41" t="n">
+      <c r="E23" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e19,6)</f>
         <v>0.003225</v>
       </c>
@@ -31402,19 +31423,19 @@
       <c r="A24" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="39" t="n">
+      <c r="B24" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b20,6)</f>
         <v>0.00156</v>
       </c>
-      <c r="C24" s="40" t="n">
+      <c r="C24" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d20,6)</f>
         <v>0.001711</v>
       </c>
-      <c r="D24" s="40" t="n">
+      <c r="D24" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c20,6)</f>
         <v>0.001661</v>
       </c>
-      <c r="E24" s="41" t="n">
+      <c r="E24" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e20,6)</f>
         <v>0.002715</v>
       </c>
@@ -31423,19 +31444,19 @@
       <c r="A25" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B25" s="39" t="n">
+      <c r="B25" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b21,6)</f>
         <v>0.00165</v>
       </c>
-      <c r="C25" s="40" t="n">
+      <c r="C25" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d21,6)</f>
         <v>0.002388</v>
       </c>
-      <c r="D25" s="40" t="n">
+      <c r="D25" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c21,6)</f>
         <v>0.001631</v>
       </c>
-      <c r="E25" s="41" t="n">
+      <c r="E25" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e21,6)</f>
         <v>0.002413</v>
       </c>
@@ -31444,19 +31465,19 @@
       <c r="A26" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="39" t="n">
+      <c r="B26" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b22,6)</f>
         <v>0.000853</v>
       </c>
-      <c r="C26" s="40" t="n">
+      <c r="C26" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d22,6)</f>
         <v>0.000793</v>
       </c>
-      <c r="D26" s="40" t="n">
+      <c r="D26" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c22,6)</f>
         <v>0.000863</v>
       </c>
-      <c r="E26" s="41" t="n">
+      <c r="E26" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e22,6)</f>
         <v>0.000877</v>
       </c>
@@ -31465,19 +31486,19 @@
       <c r="A27" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="39" t="n">
+      <c r="B27" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b23,6)</f>
         <v>0.000241</v>
       </c>
-      <c r="C27" s="40" t="n">
+      <c r="C27" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d23,6)</f>
         <v>0.000252</v>
       </c>
-      <c r="D27" s="40" t="n">
+      <c r="D27" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c23,6)</f>
         <v>0.001229</v>
       </c>
-      <c r="E27" s="41" t="n">
+      <c r="E27" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e23,6)</f>
         <v>0.000793</v>
       </c>
@@ -31486,19 +31507,19 @@
       <c r="A28" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="39" t="n">
+      <c r="B28" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b24,6)</f>
         <v>0.000346</v>
       </c>
-      <c r="C28" s="40" t="n">
+      <c r="C28" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d24,6)</f>
         <v>0.000526</v>
       </c>
-      <c r="D28" s="40" t="n">
+      <c r="D28" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c24,6)</f>
         <v>0.000592</v>
       </c>
-      <c r="E28" s="41" t="n">
+      <c r="E28" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e24,6)</f>
         <v>0.000688</v>
       </c>
@@ -31507,19 +31528,19 @@
       <c r="A29" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="39" t="n">
+      <c r="B29" s="41" t="n">
         <f aca="false">ROUND([53]output_table!b25,6)</f>
         <v>0.000236</v>
       </c>
-      <c r="C29" s="40" t="n">
+      <c r="C29" s="42" t="n">
         <f aca="false">ROUND([53]output_table!d25,6)</f>
         <v>0.000184</v>
       </c>
-      <c r="D29" s="40" t="n">
+      <c r="D29" s="42" t="n">
         <f aca="false">ROUND([53]output_table!c25,6)</f>
         <v>0.000595</v>
       </c>
-      <c r="E29" s="41" t="n">
+      <c r="E29" s="43" t="n">
         <f aca="false">ROUND([53]output_table!e25,6)</f>
         <v>0.000362</v>
       </c>
@@ -31528,19 +31549,19 @@
       <c r="A30" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="45" t="n">
         <f aca="false">ROUND([53]output_table!b26,6)</f>
         <v>0.000262</v>
       </c>
-      <c r="C30" s="44" t="n">
+      <c r="C30" s="46" t="n">
         <f aca="false">ROUND([53]output_table!d26,6)</f>
         <v>0.000358</v>
       </c>
-      <c r="D30" s="44" t="n">
+      <c r="D30" s="46" t="n">
         <f aca="false">ROUND([53]output_table!c26,6)</f>
         <v>0.000266</v>
       </c>
-      <c r="E30" s="45" t="n">
+      <c r="E30" s="47" t="n">
         <f aca="false">ROUND([53]output_table!e26,6)</f>
         <v>0.000337</v>
       </c>
@@ -31598,7 +31619,7 @@
       <c r="C2" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="48" t="s">
         <v>132</v>
       </c>
       <c r="K2" s="0" t="s">
@@ -31676,22 +31697,22 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="46"/>
+      <c r="B9" s="48"/>
       <c r="K9" s="0" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="46"/>
+      <c r="B10" s="48"/>
       <c r="K10" s="0" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="46"/>
+      <c r="B11" s="48"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="46"/>
+      <c r="B12" s="48"/>
       <c r="K12" s="0" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
New EOS Table 8
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -23,6 +23,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1103,7 +1104,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1113,277 +1114,566 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="F2">
-            <v>-4.24700584377045</v>
+            <v>-4.37331057212242</v>
           </cell>
           <cell r="G2">
-            <v>-3.22610856623628</v>
+            <v>0.21949184856248</v>
           </cell>
           <cell r="H2">
-            <v>-1.02089727753415</v>
+            <v>-4.5928024206849</v>
           </cell>
         </row>
         <row r="3">
           <cell r="F3">
-            <v>-52.9324518043044</v>
+            <v>-51.3099050414287</v>
           </cell>
           <cell r="G3">
-            <v>-52.5684229312778</v>
+            <v>-59.4441644736992</v>
           </cell>
           <cell r="H3">
-            <v>-0.364028873026663</v>
+            <v>8.13425943227054</v>
           </cell>
         </row>
         <row r="4">
           <cell r="F4">
-            <v>-73.0967524165371</v>
+            <v>-72.2214345607101</v>
           </cell>
           <cell r="G4">
-            <v>-59.8153703442266</v>
+            <v>-48.4993181771023</v>
           </cell>
           <cell r="H4">
-            <v>-13.2813820723105</v>
+            <v>-23.7221163836077</v>
           </cell>
         </row>
         <row r="5">
           <cell r="F5">
-            <v>-74.5232982923199</v>
+            <v>-74.5255934972134</v>
           </cell>
           <cell r="G5">
-            <v>-48.1591100675098</v>
+            <v>-52.3223241407493</v>
           </cell>
           <cell r="H5">
-            <v>-26.3641882248101</v>
+            <v>-22.2032693564641</v>
           </cell>
         </row>
         <row r="6">
           <cell r="F6">
-            <v>2.23985746888382</v>
+            <v>2.58721911279002</v>
           </cell>
           <cell r="G6">
-            <v>-9.50799908540213</v>
+            <v>-4.94567543537128</v>
           </cell>
           <cell r="H6">
-            <v>11.747856554286</v>
+            <v>7.53289454816127</v>
           </cell>
         </row>
         <row r="7">
           <cell r="F7">
-            <v>-31.7588698120711</v>
+            <v>-37.0915028133695</v>
           </cell>
           <cell r="G7">
-            <v>-128.44176558061</v>
+            <v>-130.91611222525</v>
           </cell>
           <cell r="H7">
-            <v>96.6828957685386</v>
+            <v>93.8246094118801</v>
           </cell>
         </row>
         <row r="8">
           <cell r="F8">
-            <v>-80.3567379627799</v>
+            <v>-80.2448798269329</v>
           </cell>
           <cell r="G8">
-            <v>-9.97227752337863</v>
+            <v>-13.5050976462384</v>
           </cell>
           <cell r="H8">
-            <v>-70.3844604394012</v>
+            <v>-66.7397821806945</v>
           </cell>
         </row>
         <row r="9">
           <cell r="F9">
-            <v>-38.2407366147895</v>
+            <v>-38.551485474784</v>
           </cell>
           <cell r="G9">
-            <v>-30.8356913932688</v>
+            <v>-28.6298828956188</v>
           </cell>
           <cell r="H9">
-            <v>-7.40504522152075</v>
+            <v>-9.92160257916519</v>
           </cell>
         </row>
         <row r="10">
           <cell r="F10">
-            <v>-20.6210356016845</v>
+            <v>-21.9039232776394</v>
           </cell>
           <cell r="G10">
-            <v>31.1083040428914</v>
+            <v>37.8334681910329</v>
           </cell>
           <cell r="H10">
-            <v>-51.729339644576</v>
+            <v>-59.7373914686722</v>
           </cell>
         </row>
         <row r="11">
           <cell r="F11">
-            <v>-41.3753993163408</v>
+            <v>-43.6721162441733</v>
           </cell>
           <cell r="G11">
-            <v>-1.69281500344195</v>
+            <v>-8.70472459793691</v>
           </cell>
           <cell r="H11">
-            <v>-39.6825843128989</v>
+            <v>-34.9673916462364</v>
           </cell>
         </row>
         <row r="12">
           <cell r="F12">
-            <v>-42.4498684100269</v>
+            <v>-30.1542399704959</v>
           </cell>
           <cell r="G12">
-            <v>-26.7806346707347</v>
+            <v>31.3868745623727</v>
           </cell>
           <cell r="H12">
-            <v>-15.6692337392926</v>
+            <v>-61.5411145328686</v>
           </cell>
         </row>
         <row r="13">
           <cell r="F13">
-            <v>-35.0449390197793</v>
+            <v>-32.8391702315125</v>
           </cell>
           <cell r="G13">
-            <v>-46.3869105352978</v>
+            <v>-29.3304594133641</v>
           </cell>
           <cell r="H13">
-            <v>11.3419715155185</v>
+            <v>-3.50871081814841</v>
           </cell>
         </row>
         <row r="14">
           <cell r="F14">
-            <v>-57.3673515037132</v>
+            <v>-58.2340883173942</v>
           </cell>
           <cell r="G14">
-            <v>-0.48314377495887</v>
+            <v>-29.7507633068765</v>
           </cell>
           <cell r="H14">
-            <v>-56.8842077287543</v>
+            <v>-28.4833250105177</v>
           </cell>
         </row>
         <row r="15">
           <cell r="F15">
-            <v>-25.8494667697873</v>
+            <v>-26.9383213720629</v>
           </cell>
           <cell r="G15">
-            <v>46.0021152751505</v>
+            <v>37.648985254093</v>
           </cell>
           <cell r="H15">
-            <v>-71.8515820449378</v>
+            <v>-64.5873066261559</v>
           </cell>
         </row>
         <row r="16">
           <cell r="F16">
-            <v>-1.61594426556377</v>
+            <v>-3.60386504403561</v>
           </cell>
           <cell r="G16">
-            <v>-5.88306081812264</v>
+            <v>4.69963427020947</v>
           </cell>
           <cell r="H16">
-            <v>4.26711655255885</v>
+            <v>-8.30349931424506</v>
           </cell>
         </row>
         <row r="17">
           <cell r="F17">
-            <v>-70.9495607886844</v>
+            <v>-69.0387027150459</v>
           </cell>
           <cell r="G17">
-            <v>-43.5065162688841</v>
+            <v>-29.3274092603577</v>
           </cell>
           <cell r="H17">
-            <v>-27.4430445198004</v>
+            <v>-39.7112934546882</v>
           </cell>
         </row>
         <row r="18">
           <cell r="F18">
-            <v>-74.2024908691538</v>
+            <v>-74.2295154959689</v>
           </cell>
           <cell r="G18">
-            <v>-51.7202514740215</v>
+            <v>-47.4839954214155</v>
           </cell>
           <cell r="H18">
-            <v>-22.4822393951322</v>
+            <v>-26.7455200745534</v>
           </cell>
         </row>
         <row r="19">
           <cell r="F19">
-            <v>-29.0808287638034</v>
+            <v>-30.4808561362157</v>
           </cell>
           <cell r="G19">
-            <v>-77.1306982466794</v>
+            <v>-65.2388925426207</v>
           </cell>
           <cell r="H19">
-            <v>48.049869482876</v>
+            <v>34.758036406405</v>
           </cell>
         </row>
         <row r="20">
           <cell r="F20">
-            <v>-13.606161287555</v>
+            <v>-14.1161374258826</v>
           </cell>
           <cell r="G20">
-            <v>-7.49759418631569</v>
+            <v>-14.3998539480107</v>
           </cell>
           <cell r="H20">
-            <v>-6.10856710123939</v>
+            <v>0.283716522128082</v>
           </cell>
         </row>
         <row r="21">
           <cell r="F21">
-            <v>3.84977636789347</v>
+            <v>3.489981441953</v>
           </cell>
           <cell r="G21">
-            <v>-8.97500143405787</v>
+            <v>-7.6898003621075</v>
           </cell>
           <cell r="H21">
-            <v>12.8247778019513</v>
+            <v>11.1797818040605</v>
           </cell>
         </row>
         <row r="22">
           <cell r="F22">
-            <v>2.80313079055405</v>
+            <v>3.12192397724355</v>
           </cell>
           <cell r="G22">
-            <v>-228.517426773814</v>
+            <v>-25.0600070513189</v>
           </cell>
           <cell r="H22">
-            <v>231.320557564368</v>
+            <v>28.1819310285625</v>
           </cell>
         </row>
         <row r="23">
           <cell r="F23">
-            <v>-81.732145531497</v>
+            <v>-81.3859372391022</v>
           </cell>
           <cell r="G23">
-            <v>-26.5044535611909</v>
+            <v>-28.6303682633693</v>
           </cell>
           <cell r="H23">
-            <v>-55.227691970306</v>
+            <v>-52.7555689757329</v>
           </cell>
         </row>
         <row r="24">
           <cell r="F24">
-            <v>-45.6163092023758</v>
+            <v>-46.4623838746426</v>
           </cell>
           <cell r="G24">
-            <v>-7.11657566882191</v>
+            <v>13.1848326449393</v>
           </cell>
           <cell r="H24">
-            <v>-38.4997335335539</v>
+            <v>-59.6472165195818</v>
           </cell>
         </row>
         <row r="25">
           <cell r="F25">
-            <v>-59.0402947071121</v>
+            <v>-59.79706852728</v>
           </cell>
           <cell r="G25">
-            <v>5.68946935205537</v>
+            <v>5.25656223697922</v>
           </cell>
           <cell r="H25">
-            <v>-64.7297640591674</v>
+            <v>-65.0536307642592</v>
           </cell>
         </row>
         <row r="26">
           <cell r="F26">
-            <v>-0.351835440384865</v>
+            <v>0.117395300848192</v>
           </cell>
           <cell r="G26">
-            <v>3.58040250822731</v>
+            <v>7.53718047506602</v>
           </cell>
           <cell r="H26">
-            <v>-3.93223794861215</v>
+            <v>-7.41978517421784</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="output_table"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="F2">
+            <v>-2.31987491526708</v>
+          </cell>
+          <cell r="G2">
+            <v>-0.635755623291128</v>
+          </cell>
+          <cell r="H2">
+            <v>-1.68411929197596</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="F3">
+            <v>-37.7089679430125</v>
+          </cell>
+          <cell r="G3">
+            <v>-102.886742958135</v>
+          </cell>
+          <cell r="H3">
+            <v>65.1777750151224</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="F4">
+            <v>-62.8618689270968</v>
+          </cell>
+          <cell r="G4">
+            <v>-67.7648065904077</v>
+          </cell>
+          <cell r="H4">
+            <v>4.90293766331088</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="F5">
+            <v>-67.7642773482324</v>
+          </cell>
+          <cell r="G5">
+            <v>-76.9031683010256</v>
+          </cell>
+          <cell r="H5">
+            <v>9.13889095279318</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="F6">
+            <v>0.385757162658495</v>
+          </cell>
+          <cell r="G6">
+            <v>-0.132035071272213</v>
+          </cell>
+          <cell r="H6">
+            <v>0.517792233930708</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="F7">
+            <v>-35.0071531786577</v>
+          </cell>
+          <cell r="G7">
+            <v>-32.8346733353409</v>
+          </cell>
+          <cell r="H7">
+            <v>-2.17247984331684</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="F8">
+            <v>-82.2221406360923</v>
+          </cell>
+          <cell r="G8">
+            <v>-41.9110620037622</v>
+          </cell>
+          <cell r="H8">
+            <v>-40.3110786323301</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="F9">
+            <v>-38.6951169846288</v>
+          </cell>
+          <cell r="G9">
+            <v>-48.7433144736645</v>
+          </cell>
+          <cell r="H9">
+            <v>10.0481974890357</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="F10">
+            <v>-21.6766231712592</v>
+          </cell>
+          <cell r="G10">
+            <v>20.2977247668418</v>
+          </cell>
+          <cell r="H10">
+            <v>-41.974347938101</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="F11">
+            <v>-61.9072501389762</v>
+          </cell>
+          <cell r="G11">
+            <v>-85.2075934332299</v>
+          </cell>
+          <cell r="H11">
+            <v>23.3003432942536</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="F12">
+            <v>-9.87829407125928</v>
+          </cell>
+          <cell r="G12">
+            <v>14.0664425936309</v>
+          </cell>
+          <cell r="H12">
+            <v>-23.9447366648902</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="F13">
+            <v>-6.85891474864828</v>
+          </cell>
+          <cell r="G13">
+            <v>-1.99049729104541</v>
+          </cell>
+          <cell r="H13">
+            <v>-4.86841745760287</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="F14">
+            <v>-59.4397653718879</v>
+          </cell>
+          <cell r="G14">
+            <v>-44.8937456946869</v>
+          </cell>
+          <cell r="H14">
+            <v>-14.546019677201</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="F15">
+            <v>-22.9194878821356</v>
+          </cell>
+          <cell r="G15">
+            <v>19.4174150285038</v>
+          </cell>
+          <cell r="H15">
+            <v>-42.3369029106393</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="F16">
+            <v>-5.29492963578905</v>
+          </cell>
+          <cell r="G16">
+            <v>1.17891457658208</v>
+          </cell>
+          <cell r="H16">
+            <v>-6.47384421237113</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="F17">
+            <v>-44.4873338410454</v>
+          </cell>
+          <cell r="G17">
+            <v>-46.6262482586029</v>
+          </cell>
+          <cell r="H17">
+            <v>2.13891441755751</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="F18">
+            <v>-72.1798332348372</v>
+          </cell>
+          <cell r="G18">
+            <v>-93.6491755004949</v>
+          </cell>
+          <cell r="H18">
+            <v>21.4693422656577</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="F19">
+            <v>-40.1973497577248</v>
+          </cell>
+          <cell r="G19">
+            <v>-58.2398549258541</v>
+          </cell>
+          <cell r="H19">
+            <v>18.0425051681294</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="F20">
+            <v>1.27998798918097</v>
+          </cell>
+          <cell r="G20">
+            <v>-58.969312210821</v>
+          </cell>
+          <cell r="H20">
+            <v>60.2493002000019</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="F21">
+            <v>-1.16864157459739</v>
+          </cell>
+          <cell r="G21">
+            <v>-2.18118993205592</v>
+          </cell>
+          <cell r="H21">
+            <v>1.01254835745855</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="F22">
+            <v>0.44376438251493</v>
+          </cell>
+          <cell r="G22">
+            <v>4.83413357500981</v>
+          </cell>
+          <cell r="H22">
+            <v>-4.39036919249488</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="F23">
+            <v>-77.1033603695931</v>
+          </cell>
+          <cell r="G23">
+            <v>-52.4719082945895</v>
+          </cell>
+          <cell r="H23">
+            <v>-24.6314520750036</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="F24">
+            <v>-32.6225959701779</v>
+          </cell>
+          <cell r="G24">
+            <v>2.19990903450105</v>
+          </cell>
+          <cell r="H24">
+            <v>-34.822505004679</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="F25">
+            <v>-60.0713929491941</v>
+          </cell>
+          <cell r="G25">
+            <v>-39.7223530120159</v>
+          </cell>
+          <cell r="H25">
+            <v>-20.3490399371782</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="F26">
+            <v>-0.575060343014248</v>
+          </cell>
+          <cell r="G26">
+            <v>1.09074064910073</v>
+          </cell>
+          <cell r="H26">
+            <v>-1.66580099211498</v>
           </cell>
         </row>
       </sheetData>
@@ -29848,7 +30138,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29865,20 +30155,20 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="str">
-        <f aca="false">CONCATENATE("Title: Changes in average volatility due to measured changes in trade barriers, alternative calibrations (",_xlfn.UNICHAR(963), " = 0.4 and ",_xlfn.UNICHAR(963), " = 1.3)")</f>
-        <v>Title: Changes in average volatility due to measured changes in trade barriers, alternative calibrations (σ = 0.4 and σ = 1.3)</v>
+        <f aca="false">CONCATENATE("Title: Changes in average volatility due to measured changes in trade barriers, alternative calibrations (",_xlfn.UNICHAR(963), " = 0.5 and ",_xlfn.UNICHAR(963), " = 1.5)")</f>
+        <v>Title: Changes in average volatility due to measured changes in trade barriers, alternative calibrations (σ = 0.5 and σ = 1.5)</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="30" t="str">
-        <f aca="false">CONCATENATE(_xlfn.UNICHAR(963)," = 0.4")</f>
-        <v>σ = 0.4</v>
+        <f aca="false">CONCATENATE(_xlfn.UNICHAR(963)," = 0.5")</f>
+        <v>σ = 0.5</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30" t="str">
-        <f aca="false">CONCATENATE(_xlfn.UNICHAR(963)," = 1.3")</f>
-        <v>σ = 1.3</v>
+        <f aca="false">CONCATENATE(_xlfn.UNICHAR(963)," = 1.5")</f>
+        <v>σ = 1.5</v>
       </c>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
@@ -29909,28 +30199,28 @@
         <v>91</v>
       </c>
       <c r="B7" s="17" t="n">
-        <f aca="false">[27]output_table!F2/100</f>
-        <v>-0.0424700584377045</v>
+        <f aca="false">[15]output_table!F2/100</f>
+        <v>-0.0437331057212242</v>
       </c>
       <c r="C7" s="18" t="n">
-        <f aca="false">[27]output_table!G2/100</f>
-        <v>-0.0322610856623628</v>
+        <f aca="false">[15]output_table!G2/100</f>
+        <v>0.0021949184856248</v>
       </c>
       <c r="D7" s="19" t="n">
-        <f aca="false">[27]output_table!H2/100</f>
-        <v>-0.0102089727753415</v>
+        <f aca="false">[15]output_table!H2/100</f>
+        <v>-0.045928024206849</v>
       </c>
       <c r="E7" s="17" t="n">
-        <f aca="false">[28]output_table!f2/100</f>
-        <v>-0.0226841459627221</v>
+        <f aca="false">[16]output_table!F2/100</f>
+        <v>-0.0231987491526708</v>
       </c>
       <c r="F7" s="18" t="n">
-        <f aca="false">[28]output_table!g2/100</f>
-        <v>-0.00358432184359962</v>
+        <f aca="false">[16]output_table!G2/100</f>
+        <v>-0.00635755623291128</v>
       </c>
       <c r="G7" s="19" t="n">
-        <f aca="false">[28]output_table!h2/100</f>
-        <v>-0.0190998241191224</v>
+        <f aca="false">[16]output_table!H2/100</f>
+        <v>-0.0168411929197596</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29938,28 +30228,28 @@
         <v>92</v>
       </c>
       <c r="B8" s="21" t="n">
-        <f aca="false">[27]output_table!F3/100</f>
-        <v>-0.529324518043044</v>
+        <f aca="false">[15]output_table!F3/100</f>
+        <v>-0.513099050414287</v>
       </c>
       <c r="C8" s="22" t="n">
-        <f aca="false">[27]output_table!G3/100</f>
-        <v>-0.525684229312778</v>
+        <f aca="false">[15]output_table!G3/100</f>
+        <v>-0.594441644736992</v>
       </c>
       <c r="D8" s="23" t="n">
-        <f aca="false">[27]output_table!H3/100</f>
-        <v>-0.00364028873026663</v>
+        <f aca="false">[15]output_table!H3/100</f>
+        <v>0.0813425943227054</v>
       </c>
       <c r="E8" s="21" t="n">
-        <f aca="false">[28]output_table!f3/100</f>
-        <v>-0.405949974462572</v>
+        <f aca="false">[16]output_table!F3/100</f>
+        <v>-0.377089679430125</v>
       </c>
       <c r="F8" s="22" t="n">
-        <f aca="false">[28]output_table!g3/100</f>
-        <v>-0.958247076304075</v>
+        <f aca="false">[16]output_table!G3/100</f>
+        <v>-1.02886742958135</v>
       </c>
       <c r="G8" s="23" t="n">
-        <f aca="false">[28]output_table!h3/100</f>
-        <v>0.552297101841503</v>
+        <f aca="false">[16]output_table!H3/100</f>
+        <v>0.651777750151224</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29967,28 +30257,28 @@
         <v>93</v>
       </c>
       <c r="B9" s="21" t="n">
-        <f aca="false">[27]output_table!F4/100</f>
-        <v>-0.730967524165371</v>
+        <f aca="false">[15]output_table!F4/100</f>
+        <v>-0.722214345607101</v>
       </c>
       <c r="C9" s="22" t="n">
-        <f aca="false">[27]output_table!G4/100</f>
-        <v>-0.598153703442266</v>
+        <f aca="false">[15]output_table!G4/100</f>
+        <v>-0.484993181771023</v>
       </c>
       <c r="D9" s="23" t="n">
-        <f aca="false">[27]output_table!H4/100</f>
-        <v>-0.132813820723105</v>
+        <f aca="false">[15]output_table!H4/100</f>
+        <v>-0.237221163836077</v>
       </c>
       <c r="E9" s="21" t="n">
-        <f aca="false">[28]output_table!f4/100</f>
-        <v>-0.652522753856962</v>
+        <f aca="false">[16]output_table!F4/100</f>
+        <v>-0.628618689270968</v>
       </c>
       <c r="F9" s="22" t="n">
-        <f aca="false">[28]output_table!g4/100</f>
-        <v>-0.642326951122212</v>
+        <f aca="false">[16]output_table!G4/100</f>
+        <v>-0.677648065904077</v>
       </c>
       <c r="G9" s="23" t="n">
-        <f aca="false">[28]output_table!h4/100</f>
-        <v>-0.01019580273475</v>
+        <f aca="false">[16]output_table!H4/100</f>
+        <v>0.0490293766331088</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29996,28 +30286,28 @@
         <v>94</v>
       </c>
       <c r="B10" s="21" t="n">
-        <f aca="false">[27]output_table!F5/100</f>
-        <v>-0.745232982923199</v>
+        <f aca="false">[15]output_table!F5/100</f>
+        <v>-0.745255934972134</v>
       </c>
       <c r="C10" s="22" t="n">
-        <f aca="false">[27]output_table!G5/100</f>
-        <v>-0.481591100675098</v>
+        <f aca="false">[15]output_table!G5/100</f>
+        <v>-0.523223241407493</v>
       </c>
       <c r="D10" s="23" t="n">
-        <f aca="false">[27]output_table!H5/100</f>
-        <v>-0.263641882248101</v>
+        <f aca="false">[15]output_table!H5/100</f>
+        <v>-0.222032693564641</v>
       </c>
       <c r="E10" s="21" t="n">
-        <f aca="false">[28]output_table!f5/100</f>
-        <v>-0.700915836976509</v>
+        <f aca="false">[16]output_table!F5/100</f>
+        <v>-0.677642773482324</v>
       </c>
       <c r="F10" s="22" t="n">
-        <f aca="false">[28]output_table!g5/100</f>
-        <v>-0.765091950206227</v>
+        <f aca="false">[16]output_table!G5/100</f>
+        <v>-0.769031683010256</v>
       </c>
       <c r="G10" s="23" t="n">
-        <f aca="false">[28]output_table!h5/100</f>
-        <v>0.0641761132297187</v>
+        <f aca="false">[16]output_table!H5/100</f>
+        <v>0.0913889095279318</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30025,28 +30315,28 @@
         <v>95</v>
       </c>
       <c r="B11" s="21" t="n">
-        <f aca="false">[27]output_table!F6/100</f>
-        <v>0.0223985746888382</v>
+        <f aca="false">[15]output_table!F6/100</f>
+        <v>0.0258721911279002</v>
       </c>
       <c r="C11" s="22" t="n">
-        <f aca="false">[27]output_table!G6/100</f>
-        <v>-0.0950799908540213</v>
+        <f aca="false">[15]output_table!G6/100</f>
+        <v>-0.0494567543537128</v>
       </c>
       <c r="D11" s="23" t="n">
-        <f aca="false">[27]output_table!H6/100</f>
-        <v>0.11747856554286</v>
+        <f aca="false">[15]output_table!H6/100</f>
+        <v>0.0753289454816127</v>
       </c>
       <c r="E11" s="21" t="n">
-        <f aca="false">[28]output_table!f6/100</f>
-        <v>0.00634566883199406</v>
+        <f aca="false">[16]output_table!F6/100</f>
+        <v>0.00385757162658495</v>
       </c>
       <c r="F11" s="22" t="n">
-        <f aca="false">[28]output_table!g6/100</f>
-        <v>-0.000891236308778796</v>
+        <f aca="false">[16]output_table!G6/100</f>
+        <v>-0.00132035071272213</v>
       </c>
       <c r="G11" s="23" t="n">
-        <f aca="false">[28]output_table!h6/100</f>
-        <v>0.00723690514077286</v>
+        <f aca="false">[16]output_table!H6/100</f>
+        <v>0.00517792233930708</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30054,28 +30344,28 @@
         <v>96</v>
       </c>
       <c r="B12" s="21" t="n">
-        <f aca="false">[27]output_table!F7/100</f>
-        <v>-0.317588698120711</v>
+        <f aca="false">[15]output_table!F7/100</f>
+        <v>-0.370915028133695</v>
       </c>
       <c r="C12" s="22" t="n">
-        <f aca="false">[27]output_table!G7/100</f>
-        <v>-1.2844176558061</v>
+        <f aca="false">[15]output_table!G7/100</f>
+        <v>-1.3091611222525</v>
       </c>
       <c r="D12" s="23" t="n">
-        <f aca="false">[27]output_table!H7/100</f>
-        <v>0.966828957685386</v>
+        <f aca="false">[15]output_table!H7/100</f>
+        <v>0.938246094118801</v>
       </c>
       <c r="E12" s="21" t="n">
-        <f aca="false">[28]output_table!f7/100</f>
-        <v>-0.384695455364029</v>
+        <f aca="false">[16]output_table!F7/100</f>
+        <v>-0.350071531786577</v>
       </c>
       <c r="F12" s="22" t="n">
-        <f aca="false">[28]output_table!g7/100</f>
-        <v>-0.397098475070796</v>
+        <f aca="false">[16]output_table!G7/100</f>
+        <v>-0.328346733353409</v>
       </c>
       <c r="G12" s="23" t="n">
-        <f aca="false">[28]output_table!h7/100</f>
-        <v>0.0124030197067676</v>
+        <f aca="false">[16]output_table!H7/100</f>
+        <v>-0.0217247984331684</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30083,28 +30373,28 @@
         <v>97</v>
       </c>
       <c r="B13" s="21" t="n">
-        <f aca="false">[27]output_table!F8/100</f>
-        <v>-0.803567379627799</v>
+        <f aca="false">[15]output_table!F8/100</f>
+        <v>-0.802448798269329</v>
       </c>
       <c r="C13" s="22" t="n">
-        <f aca="false">[27]output_table!G8/100</f>
-        <v>-0.0997227752337863</v>
+        <f aca="false">[15]output_table!G8/100</f>
+        <v>-0.135050976462384</v>
       </c>
       <c r="D13" s="23" t="n">
-        <f aca="false">[27]output_table!H8/100</f>
-        <v>-0.703844604394012</v>
+        <f aca="false">[15]output_table!H8/100</f>
+        <v>-0.667397821806945</v>
       </c>
       <c r="E13" s="21" t="n">
-        <f aca="false">[28]output_table!f8/100</f>
-        <v>-0.813419436809039</v>
+        <f aca="false">[16]output_table!F8/100</f>
+        <v>-0.822221406360923</v>
       </c>
       <c r="F13" s="22" t="n">
-        <f aca="false">[28]output_table!g8/100</f>
-        <v>-0.348895516108597</v>
+        <f aca="false">[16]output_table!G8/100</f>
+        <v>-0.419110620037622</v>
       </c>
       <c r="G13" s="23" t="n">
-        <f aca="false">[28]output_table!h8/100</f>
-        <v>-0.464523920700442</v>
+        <f aca="false">[16]output_table!H8/100</f>
+        <v>-0.403110786323301</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30112,28 +30402,28 @@
         <v>98</v>
       </c>
       <c r="B14" s="21" t="n">
-        <f aca="false">[27]output_table!F9/100</f>
-        <v>-0.382407366147895</v>
+        <f aca="false">[15]output_table!F9/100</f>
+        <v>-0.38551485474784</v>
       </c>
       <c r="C14" s="22" t="n">
-        <f aca="false">[27]output_table!G9/100</f>
-        <v>-0.308356913932688</v>
+        <f aca="false">[15]output_table!G9/100</f>
+        <v>-0.286298828956188</v>
       </c>
       <c r="D14" s="23" t="n">
-        <f aca="false">[27]output_table!H9/100</f>
-        <v>-0.0740504522152075</v>
+        <f aca="false">[15]output_table!H9/100</f>
+        <v>-0.0992160257916519</v>
       </c>
       <c r="E14" s="21" t="n">
-        <f aca="false">[28]output_table!f9/100</f>
-        <v>-0.384804139596221</v>
+        <f aca="false">[16]output_table!F9/100</f>
+        <v>-0.386951169846288</v>
       </c>
       <c r="F14" s="22" t="n">
-        <f aca="false">[28]output_table!g9/100</f>
-        <v>-0.435369783333816</v>
+        <f aca="false">[16]output_table!G9/100</f>
+        <v>-0.487433144736644</v>
       </c>
       <c r="G14" s="23" t="n">
-        <f aca="false">[28]output_table!h9/100</f>
-        <v>0.050565643737595</v>
+        <f aca="false">[16]output_table!H9/100</f>
+        <v>0.100481974890357</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30141,28 +30431,28 @@
         <v>99</v>
       </c>
       <c r="B15" s="21" t="n">
-        <f aca="false">[27]output_table!F10/100</f>
-        <v>-0.206210356016845</v>
+        <f aca="false">[15]output_table!F10/100</f>
+        <v>-0.219039232776394</v>
       </c>
       <c r="C15" s="22" t="n">
-        <f aca="false">[27]output_table!G10/100</f>
-        <v>0.311083040428914</v>
+        <f aca="false">[15]output_table!G10/100</f>
+        <v>0.378334681910329</v>
       </c>
       <c r="D15" s="23" t="n">
-        <f aca="false">[27]output_table!H10/100</f>
-        <v>-0.51729339644576</v>
+        <f aca="false">[15]output_table!H10/100</f>
+        <v>-0.597373914686722</v>
       </c>
       <c r="E15" s="21" t="n">
-        <f aca="false">[28]output_table!f10/100</f>
-        <v>-0.234523959421473</v>
+        <f aca="false">[16]output_table!F10/100</f>
+        <v>-0.216766231712592</v>
       </c>
       <c r="F15" s="22" t="n">
-        <f aca="false">[28]output_table!g10/100</f>
-        <v>0.23455844346093</v>
+        <f aca="false">[16]output_table!G10/100</f>
+        <v>0.202977247668418</v>
       </c>
       <c r="G15" s="23" t="n">
-        <f aca="false">[28]output_table!h10/100</f>
-        <v>-0.469082402882403</v>
+        <f aca="false">[16]output_table!H10/100</f>
+        <v>-0.41974347938101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30170,28 +30460,28 @@
         <v>100</v>
       </c>
       <c r="B16" s="21" t="n">
-        <f aca="false">[27]output_table!F11/100</f>
-        <v>-0.413753993163408</v>
+        <f aca="false">[15]output_table!F11/100</f>
+        <v>-0.436721162441733</v>
       </c>
       <c r="C16" s="22" t="n">
-        <f aca="false">[27]output_table!G11/100</f>
-        <v>-0.0169281500344195</v>
+        <f aca="false">[15]output_table!G11/100</f>
+        <v>-0.0870472459793691</v>
       </c>
       <c r="D16" s="23" t="n">
-        <f aca="false">[27]output_table!H11/100</f>
-        <v>-0.396825843128989</v>
+        <f aca="false">[15]output_table!H11/100</f>
+        <v>-0.349673916462364</v>
       </c>
       <c r="E16" s="21" t="n">
-        <f aca="false">[28]output_table!f11/100</f>
-        <v>-0.587461029005024</v>
+        <f aca="false">[16]output_table!F11/100</f>
+        <v>-0.619072501389762</v>
       </c>
       <c r="F16" s="22" t="n">
-        <f aca="false">[28]output_table!g11/100</f>
-        <v>-0.698822002943098</v>
+        <f aca="false">[16]output_table!G11/100</f>
+        <v>-0.852075934332298</v>
       </c>
       <c r="G16" s="23" t="n">
-        <f aca="false">[28]output_table!h11/100</f>
-        <v>0.111360973938074</v>
+        <f aca="false">[16]output_table!H11/100</f>
+        <v>0.233003432942536</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30199,28 +30489,28 @@
         <v>101</v>
       </c>
       <c r="B17" s="21" t="n">
-        <f aca="false">[27]output_table!F12/100</f>
-        <v>-0.424498684100269</v>
+        <f aca="false">[15]output_table!F12/100</f>
+        <v>-0.301542399704959</v>
       </c>
       <c r="C17" s="22" t="n">
-        <f aca="false">[27]output_table!G12/100</f>
-        <v>-0.267806346707347</v>
+        <f aca="false">[15]output_table!G12/100</f>
+        <v>0.313868745623727</v>
       </c>
       <c r="D17" s="23" t="n">
-        <f aca="false">[27]output_table!H12/100</f>
-        <v>-0.156692337392926</v>
+        <f aca="false">[15]output_table!H12/100</f>
+        <v>-0.615411145328686</v>
       </c>
       <c r="E17" s="21" t="n">
-        <f aca="false">[28]output_table!f12/100</f>
-        <v>-0.181133296014505</v>
+        <f aca="false">[16]output_table!F12/100</f>
+        <v>-0.0987829407125928</v>
       </c>
       <c r="F17" s="22" t="n">
-        <f aca="false">[28]output_table!g12/100</f>
-        <v>0.209230382439203</v>
+        <f aca="false">[16]output_table!G12/100</f>
+        <v>0.140664425936309</v>
       </c>
       <c r="G17" s="23" t="n">
-        <f aca="false">[28]output_table!h12/100</f>
-        <v>-0.390363678453708</v>
+        <f aca="false">[16]output_table!H12/100</f>
+        <v>-0.239447366648902</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30228,28 +30518,28 @@
         <v>102</v>
       </c>
       <c r="B18" s="21" t="n">
-        <f aca="false">[27]output_table!F13/100</f>
-        <v>-0.350449390197793</v>
+        <f aca="false">[15]output_table!F13/100</f>
+        <v>-0.328391702315125</v>
       </c>
       <c r="C18" s="22" t="n">
-        <f aca="false">[27]output_table!G13/100</f>
-        <v>-0.463869105352978</v>
+        <f aca="false">[15]output_table!G13/100</f>
+        <v>-0.293304594133641</v>
       </c>
       <c r="D18" s="23" t="n">
-        <f aca="false">[27]output_table!H13/100</f>
-        <v>0.113419715155185</v>
+        <f aca="false">[15]output_table!H13/100</f>
+        <v>-0.0350871081814841</v>
       </c>
       <c r="E18" s="21" t="n">
-        <f aca="false">[28]output_table!f13/100</f>
-        <v>-0.104202007484901</v>
+        <f aca="false">[16]output_table!F13/100</f>
+        <v>-0.0685891474864828</v>
       </c>
       <c r="F18" s="22" t="n">
-        <f aca="false">[28]output_table!g13/100</f>
-        <v>-0.0400271634864455</v>
+        <f aca="false">[16]output_table!G13/100</f>
+        <v>-0.0199049729104541</v>
       </c>
       <c r="G18" s="23" t="n">
-        <f aca="false">[28]output_table!h13/100</f>
-        <v>-0.0641748439984555</v>
+        <f aca="false">[16]output_table!H13/100</f>
+        <v>-0.0486841745760287</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30257,28 +30547,28 @@
         <v>103</v>
       </c>
       <c r="B19" s="21" t="n">
-        <f aca="false">[27]output_table!F14/100</f>
-        <v>-0.573673515037132</v>
+        <f aca="false">[15]output_table!F14/100</f>
+        <v>-0.582340883173942</v>
       </c>
       <c r="C19" s="22" t="n">
-        <f aca="false">[27]output_table!G14/100</f>
-        <v>-0.0048314377495887</v>
+        <f aca="false">[15]output_table!G14/100</f>
+        <v>-0.297507633068765</v>
       </c>
       <c r="D19" s="23" t="n">
-        <f aca="false">[27]output_table!H14/100</f>
-        <v>-0.568842077287542</v>
+        <f aca="false">[15]output_table!H14/100</f>
+        <v>-0.284833250105177</v>
       </c>
       <c r="E19" s="21" t="n">
-        <f aca="false">[28]output_table!f14/100</f>
-        <v>-0.604010098896906</v>
+        <f aca="false">[16]output_table!F14/100</f>
+        <v>-0.594397653718879</v>
       </c>
       <c r="F19" s="22" t="n">
-        <f aca="false">[28]output_table!g14/100</f>
-        <v>-0.472987068150296</v>
+        <f aca="false">[16]output_table!G14/100</f>
+        <v>-0.448937456946869</v>
       </c>
       <c r="G19" s="23" t="n">
-        <f aca="false">[28]output_table!h14/100</f>
-        <v>-0.13102303074661</v>
+        <f aca="false">[16]output_table!H14/100</f>
+        <v>-0.14546019677201</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30286,28 +30576,28 @@
         <v>104</v>
       </c>
       <c r="B20" s="21" t="n">
-        <f aca="false">[27]output_table!F15/100</f>
-        <v>-0.258494667697873</v>
+        <f aca="false">[15]output_table!F15/100</f>
+        <v>-0.269383213720629</v>
       </c>
       <c r="C20" s="22" t="n">
-        <f aca="false">[27]output_table!G15/100</f>
-        <v>0.460021152751505</v>
+        <f aca="false">[15]output_table!G15/100</f>
+        <v>0.37648985254093</v>
       </c>
       <c r="D20" s="23" t="n">
-        <f aca="false">[27]output_table!H15/100</f>
-        <v>-0.718515820449378</v>
+        <f aca="false">[15]output_table!H15/100</f>
+        <v>-0.645873066261559</v>
       </c>
       <c r="E20" s="21" t="n">
-        <f aca="false">[28]output_table!f15/100</f>
-        <v>-0.25125356500322</v>
+        <f aca="false">[16]output_table!F15/100</f>
+        <v>-0.229194878821356</v>
       </c>
       <c r="F20" s="22" t="n">
-        <f aca="false">[28]output_table!g15/100</f>
-        <v>0.226995332003587</v>
+        <f aca="false">[16]output_table!G15/100</f>
+        <v>0.194174150285038</v>
       </c>
       <c r="G20" s="23" t="n">
-        <f aca="false">[28]output_table!h15/100</f>
-        <v>-0.478248897006807</v>
+        <f aca="false">[16]output_table!H15/100</f>
+        <v>-0.423369029106393</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30315,28 +30605,28 @@
         <v>105</v>
       </c>
       <c r="B21" s="21" t="n">
-        <f aca="false">[27]output_table!F16/100</f>
-        <v>-0.0161594426556377</v>
+        <f aca="false">[15]output_table!F16/100</f>
+        <v>-0.0360386504403561</v>
       </c>
       <c r="C21" s="22" t="n">
-        <f aca="false">[27]output_table!G16/100</f>
-        <v>-0.0588306081812264</v>
+        <f aca="false">[15]output_table!G16/100</f>
+        <v>0.0469963427020947</v>
       </c>
       <c r="D21" s="23" t="n">
-        <f aca="false">[27]output_table!H16/100</f>
-        <v>0.0426711655255885</v>
+        <f aca="false">[15]output_table!H16/100</f>
+        <v>-0.0830349931424506</v>
       </c>
       <c r="E21" s="21" t="n">
-        <f aca="false">[28]output_table!f16/100</f>
-        <v>-0.0550849136631305</v>
+        <f aca="false">[16]output_table!F16/100</f>
+        <v>-0.0529492963578905</v>
       </c>
       <c r="F21" s="22" t="n">
-        <f aca="false">[28]output_table!g16/100</f>
-        <v>0.0265979324750983</v>
+        <f aca="false">[16]output_table!G16/100</f>
+        <v>0.0117891457658208</v>
       </c>
       <c r="G21" s="23" t="n">
-        <f aca="false">[28]output_table!h16/100</f>
-        <v>-0.0816828461382288</v>
+        <f aca="false">[16]output_table!H16/100</f>
+        <v>-0.0647384421237113</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30344,28 +30634,28 @@
         <v>106</v>
       </c>
       <c r="B22" s="21" t="n">
-        <f aca="false">[27]output_table!F17/100</f>
-        <v>-0.709495607886844</v>
+        <f aca="false">[15]output_table!F17/100</f>
+        <v>-0.690387027150459</v>
       </c>
       <c r="C22" s="22" t="n">
-        <f aca="false">[27]output_table!G17/100</f>
-        <v>-0.43506516268884</v>
+        <f aca="false">[15]output_table!G17/100</f>
+        <v>-0.293274092603577</v>
       </c>
       <c r="D22" s="23" t="n">
-        <f aca="false">[27]output_table!H17/100</f>
-        <v>-0.274430445198004</v>
+        <f aca="false">[15]output_table!H17/100</f>
+        <v>-0.397112934546882</v>
       </c>
       <c r="E22" s="21" t="n">
-        <f aca="false">[28]output_table!f17/100</f>
-        <v>-0.494343386533971</v>
+        <f aca="false">[16]output_table!F17/100</f>
+        <v>-0.444873338410454</v>
       </c>
       <c r="F22" s="22" t="n">
-        <f aca="false">[28]output_table!g17/100</f>
-        <v>-0.476337769409249</v>
+        <f aca="false">[16]output_table!G17/100</f>
+        <v>-0.466262482586029</v>
       </c>
       <c r="G22" s="23" t="n">
-        <f aca="false">[28]output_table!h17/100</f>
-        <v>-0.0180056171247219</v>
+        <f aca="false">[16]output_table!H17/100</f>
+        <v>0.0213891441755751</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30373,28 +30663,28 @@
         <v>107</v>
       </c>
       <c r="B23" s="21" t="n">
-        <f aca="false">[27]output_table!F18/100</f>
-        <v>-0.742024908691538</v>
+        <f aca="false">[15]output_table!F18/100</f>
+        <v>-0.742295154959689</v>
       </c>
       <c r="C23" s="22" t="n">
-        <f aca="false">[27]output_table!G18/100</f>
-        <v>-0.517202514740216</v>
+        <f aca="false">[15]output_table!G18/100</f>
+        <v>-0.474839954214155</v>
       </c>
       <c r="D23" s="23" t="n">
-        <f aca="false">[27]output_table!H18/100</f>
-        <v>-0.224822393951322</v>
+        <f aca="false">[15]output_table!H18/100</f>
+        <v>-0.267455200745534</v>
       </c>
       <c r="E23" s="21" t="n">
-        <f aca="false">[28]output_table!f18/100</f>
-        <v>-0.727835555843657</v>
+        <f aca="false">[16]output_table!F18/100</f>
+        <v>-0.721798332348372</v>
       </c>
       <c r="F23" s="22" t="n">
-        <f aca="false">[28]output_table!g18/100</f>
-        <v>-0.872918428432004</v>
+        <f aca="false">[16]output_table!G18/100</f>
+        <v>-0.936491755004949</v>
       </c>
       <c r="G23" s="23" t="n">
-        <f aca="false">[28]output_table!h18/100</f>
-        <v>0.145082872588347</v>
+        <f aca="false">[16]output_table!H18/100</f>
+        <v>0.214693422656577</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30402,28 +30692,28 @@
         <v>108</v>
       </c>
       <c r="B24" s="21" t="n">
-        <f aca="false">[27]output_table!F19/100</f>
-        <v>-0.290808287638034</v>
+        <f aca="false">[15]output_table!F19/100</f>
+        <v>-0.304808561362157</v>
       </c>
       <c r="C24" s="22" t="n">
-        <f aca="false">[27]output_table!G19/100</f>
-        <v>-0.771306982466794</v>
+        <f aca="false">[15]output_table!G19/100</f>
+        <v>-0.652388925426207</v>
       </c>
       <c r="D24" s="23" t="n">
-        <f aca="false">[27]output_table!H19/100</f>
-        <v>0.48049869482876</v>
+        <f aca="false">[15]output_table!H19/100</f>
+        <v>0.34758036406405</v>
       </c>
       <c r="E24" s="21" t="n">
-        <f aca="false">[28]output_table!f19/100</f>
-        <v>-0.38845609988043</v>
+        <f aca="false">[16]output_table!F19/100</f>
+        <v>-0.401973497577248</v>
       </c>
       <c r="F24" s="22" t="n">
-        <f aca="false">[28]output_table!g19/100</f>
-        <v>-0.597967373471684</v>
+        <f aca="false">[16]output_table!G19/100</f>
+        <v>-0.582398549258541</v>
       </c>
       <c r="G24" s="23" t="n">
-        <f aca="false">[28]output_table!h19/100</f>
-        <v>0.209511273591255</v>
+        <f aca="false">[16]output_table!H19/100</f>
+        <v>0.180425051681294</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30431,28 +30721,28 @@
         <v>109</v>
       </c>
       <c r="B25" s="21" t="n">
-        <f aca="false">[27]output_table!F20/100</f>
-        <v>-0.13606161287555</v>
+        <f aca="false">[15]output_table!F20/100</f>
+        <v>-0.141161374258826</v>
       </c>
       <c r="C25" s="22" t="n">
-        <f aca="false">[27]output_table!G20/100</f>
-        <v>-0.0749759418631569</v>
+        <f aca="false">[15]output_table!G20/100</f>
+        <v>-0.143998539480106</v>
       </c>
       <c r="D25" s="23" t="n">
-        <f aca="false">[27]output_table!H20/100</f>
-        <v>-0.0610856710123939</v>
+        <f aca="false">[15]output_table!H20/100</f>
+        <v>0.00283716522128082</v>
       </c>
       <c r="E25" s="21" t="n">
-        <f aca="false">[28]output_table!f20/100</f>
-        <v>-0.0123949114354937</v>
+        <f aca="false">[16]output_table!F20/100</f>
+        <v>0.0127998798918097</v>
       </c>
       <c r="F25" s="22" t="n">
-        <f aca="false">[28]output_table!g20/100</f>
-        <v>-0.52532574988439</v>
+        <f aca="false">[16]output_table!G20/100</f>
+        <v>-0.58969312210821</v>
       </c>
       <c r="G25" s="23" t="n">
-        <f aca="false">[28]output_table!h20/100</f>
-        <v>0.512930838448897</v>
+        <f aca="false">[16]output_table!H20/100</f>
+        <v>0.602493002000019</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30460,28 +30750,28 @@
         <v>110</v>
       </c>
       <c r="B26" s="21" t="n">
-        <f aca="false">[27]output_table!F21/100</f>
-        <v>0.0384977636789347</v>
+        <f aca="false">[15]output_table!F21/100</f>
+        <v>0.03489981441953</v>
       </c>
       <c r="C26" s="22" t="n">
-        <f aca="false">[27]output_table!G21/100</f>
-        <v>-0.0897500143405787</v>
+        <f aca="false">[15]output_table!G21/100</f>
+        <v>-0.076898003621075</v>
       </c>
       <c r="D26" s="23" t="n">
-        <f aca="false">[27]output_table!H21/100</f>
-        <v>0.128247778019513</v>
+        <f aca="false">[15]output_table!H21/100</f>
+        <v>0.111797818040605</v>
       </c>
       <c r="E26" s="21" t="n">
-        <f aca="false">[28]output_table!f21/100</f>
-        <v>-0.00197237766447248</v>
+        <f aca="false">[16]output_table!F21/100</f>
+        <v>-0.0116864157459739</v>
       </c>
       <c r="F26" s="22" t="n">
-        <f aca="false">[28]output_table!g21/100</f>
-        <v>-0.0301179003694763</v>
+        <f aca="false">[16]output_table!G21/100</f>
+        <v>-0.0218118993205592</v>
       </c>
       <c r="G26" s="23" t="n">
-        <f aca="false">[28]output_table!h21/100</f>
-        <v>0.028145522705004</v>
+        <f aca="false">[16]output_table!H21/100</f>
+        <v>0.0101254835745855</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30489,28 +30779,28 @@
         <v>111</v>
       </c>
       <c r="B27" s="21" t="n">
-        <f aca="false">[27]output_table!F22/100</f>
-        <v>0.0280313079055405</v>
+        <f aca="false">[15]output_table!F22/100</f>
+        <v>0.0312192397724355</v>
       </c>
       <c r="C27" s="22" t="n">
-        <f aca="false">[27]output_table!G22/100</f>
-        <v>-2.28517426773814</v>
+        <f aca="false">[15]output_table!G22/100</f>
+        <v>-0.250600070513189</v>
       </c>
       <c r="D27" s="23" t="n">
-        <f aca="false">[27]output_table!H22/100</f>
-        <v>2.31320557564368</v>
+        <f aca="false">[15]output_table!H22/100</f>
+        <v>0.281819310285625</v>
       </c>
       <c r="E27" s="21" t="n">
-        <f aca="false">[28]output_table!f22/100</f>
-        <v>-0.00605341011763756</v>
+        <f aca="false">[16]output_table!F22/100</f>
+        <v>0.0044376438251493</v>
       </c>
       <c r="F27" s="22" t="n">
-        <f aca="false">[28]output_table!g22/100</f>
-        <v>0.0255358539475986</v>
+        <f aca="false">[16]output_table!G22/100</f>
+        <v>0.0483413357500981</v>
       </c>
       <c r="G27" s="23" t="n">
-        <f aca="false">[28]output_table!h22/100</f>
-        <v>-0.0315892640652362</v>
+        <f aca="false">[16]output_table!H22/100</f>
+        <v>-0.0439036919249488</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30518,28 +30808,28 @@
         <v>112</v>
       </c>
       <c r="B28" s="21" t="n">
-        <f aca="false">[27]output_table!F23/100</f>
-        <v>-0.81732145531497</v>
+        <f aca="false">[15]output_table!F23/100</f>
+        <v>-0.813859372391022</v>
       </c>
       <c r="C28" s="22" t="n">
-        <f aca="false">[27]output_table!G23/100</f>
-        <v>-0.265044535611909</v>
+        <f aca="false">[15]output_table!G23/100</f>
+        <v>-0.286303682633693</v>
       </c>
       <c r="D28" s="23" t="n">
-        <f aca="false">[27]output_table!H23/100</f>
-        <v>-0.55227691970306</v>
+        <f aca="false">[15]output_table!H23/100</f>
+        <v>-0.527555689757329</v>
       </c>
       <c r="E28" s="21" t="n">
-        <f aca="false">[28]output_table!f23/100</f>
-        <v>-0.786782026307128</v>
+        <f aca="false">[16]output_table!F23/100</f>
+        <v>-0.771033603695931</v>
       </c>
       <c r="F28" s="22" t="n">
-        <f aca="false">[28]output_table!g23/100</f>
-        <v>-0.513190138184122</v>
+        <f aca="false">[16]output_table!G23/100</f>
+        <v>-0.524719082945895</v>
       </c>
       <c r="G28" s="23" t="n">
-        <f aca="false">[28]output_table!h23/100</f>
-        <v>-0.273591888123006</v>
+        <f aca="false">[16]output_table!H23/100</f>
+        <v>-0.246314520750036</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30547,28 +30837,28 @@
         <v>113</v>
       </c>
       <c r="B29" s="21" t="n">
-        <f aca="false">[27]output_table!F24/100</f>
-        <v>-0.456163092023758</v>
+        <f aca="false">[15]output_table!F24/100</f>
+        <v>-0.464623838746426</v>
       </c>
       <c r="C29" s="22" t="n">
-        <f aca="false">[27]output_table!G24/100</f>
-        <v>-0.0711657566882191</v>
+        <f aca="false">[15]output_table!G24/100</f>
+        <v>0.131848326449393</v>
       </c>
       <c r="D29" s="23" t="n">
-        <f aca="false">[27]output_table!H24/100</f>
-        <v>-0.384997335335539</v>
+        <f aca="false">[15]output_table!H24/100</f>
+        <v>-0.596472165195818</v>
       </c>
       <c r="E29" s="21" t="n">
-        <f aca="false">[28]output_table!f24/100</f>
-        <v>-0.360806126968098</v>
+        <f aca="false">[16]output_table!F24/100</f>
+        <v>-0.326225959701779</v>
       </c>
       <c r="F29" s="22" t="n">
-        <f aca="false">[28]output_table!g24/100</f>
-        <v>0.0365352092382854</v>
+        <f aca="false">[16]output_table!G24/100</f>
+        <v>0.0219990903450105</v>
       </c>
       <c r="G29" s="23" t="n">
-        <f aca="false">[28]output_table!h24/100</f>
-        <v>-0.397341336206383</v>
+        <f aca="false">[16]output_table!H24/100</f>
+        <v>-0.34822505004679</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30576,28 +30866,28 @@
         <v>114</v>
       </c>
       <c r="B30" s="21" t="n">
-        <f aca="false">[27]output_table!F25/100</f>
-        <v>-0.590402947071121</v>
+        <f aca="false">[15]output_table!F25/100</f>
+        <v>-0.5979706852728</v>
       </c>
       <c r="C30" s="22" t="n">
-        <f aca="false">[27]output_table!G25/100</f>
-        <v>0.0568946935205537</v>
+        <f aca="false">[15]output_table!G25/100</f>
+        <v>0.0525656223697922</v>
       </c>
       <c r="D30" s="23" t="n">
-        <f aca="false">[27]output_table!H25/100</f>
-        <v>-0.647297640591674</v>
+        <f aca="false">[15]output_table!H25/100</f>
+        <v>-0.650536307642592</v>
       </c>
       <c r="E30" s="21" t="n">
-        <f aca="false">[28]output_table!f25/100</f>
-        <v>-0.604260852771997</v>
+        <f aca="false">[16]output_table!F25/100</f>
+        <v>-0.600713929491941</v>
       </c>
       <c r="F30" s="22" t="n">
-        <f aca="false">[28]output_table!g25/100</f>
-        <v>-0.330674228555407</v>
+        <f aca="false">[16]output_table!G25/100</f>
+        <v>-0.397223530120159</v>
       </c>
       <c r="G30" s="23" t="n">
-        <f aca="false">[28]output_table!h25/100</f>
-        <v>-0.273586624216589</v>
+        <f aca="false">[16]output_table!H25/100</f>
+        <v>-0.203490399371782</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30605,28 +30895,28 @@
         <v>115</v>
       </c>
       <c r="B31" s="25" t="n">
-        <f aca="false">[27]output_table!F26/100</f>
-        <v>-0.00351835440384865</v>
+        <f aca="false">[15]output_table!F26/100</f>
+        <v>0.00117395300848192</v>
       </c>
       <c r="C31" s="26" t="n">
-        <f aca="false">[27]output_table!G26/100</f>
-        <v>0.0358040250822731</v>
+        <f aca="false">[15]output_table!G26/100</f>
+        <v>0.0753718047506602</v>
       </c>
       <c r="D31" s="27" t="n">
-        <f aca="false">[27]output_table!H26/100</f>
-        <v>-0.0393223794861215</v>
+        <f aca="false">[15]output_table!H26/100</f>
+        <v>-0.0741978517421784</v>
       </c>
       <c r="E31" s="25" t="n">
-        <f aca="false">[28]output_table!f26/100</f>
-        <v>-0.0100340647875241</v>
+        <f aca="false">[16]output_table!F26/100</f>
+        <v>-0.00575060343014248</v>
       </c>
       <c r="F31" s="26" t="n">
-        <f aca="false">[28]output_table!g26/100</f>
-        <v>0.0327454604153869</v>
+        <f aca="false">[16]output_table!G26/100</f>
+        <v>0.0109074064910073</v>
       </c>
       <c r="G31" s="27" t="n">
-        <f aca="false">[28]output_table!h26/100</f>
-        <v>-0.042779525202911</v>
+        <f aca="false">[16]output_table!H26/100</f>
+        <v>-0.0166580099211498</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30635,27 +30925,27 @@
       </c>
       <c r="B32" s="28" t="n">
         <f aca="false">AVERAGE(B7:B31)</f>
-        <v>-0.378066687838681</v>
+        <v>-0.376743167130071</v>
       </c>
       <c r="C32" s="28" t="n">
         <f aca="false">AVERAGE(C7:C31)</f>
-        <v>-0.31533661469197</v>
+        <v>-0.194444727871261</v>
       </c>
       <c r="D32" s="28" t="n">
         <f aca="false">AVERAGE(D7:D31)</f>
-        <v>-0.0627300731467108</v>
+        <v>-0.18229843925881</v>
       </c>
       <c r="E32" s="28" t="n">
         <f aca="false">AVERAGE(E7:E31)</f>
-        <v>-0.350770150239825</v>
+        <v>-0.336340289383509</v>
       </c>
       <c r="F32" s="28" t="n">
         <f aca="false">AVERAGE(F7:F31)</f>
-        <v>-0.292706980768167</v>
+        <v>-0.31707126267445</v>
       </c>
       <c r="G32" s="28" t="n">
         <f aca="false">AVERAGE(G7:G31)</f>
-        <v>-0.0580631694716576</v>
+        <v>-0.019269026709059</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>